<commit_message>
Attempting to add VadjP/N external DAC support.  It only works right now for rows 0 and 2...
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="18195" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="18195" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD Write Registers" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="242">
   <si>
     <t>Register Number</t>
   </si>
@@ -735,6 +735,15 @@
   <si>
     <t>see reg 592</t>
   </si>
+  <si>
+    <t>USE_EXTERNAL_VADJ_DACS</t>
+  </si>
+  <si>
+    <t>LSB chooses whether to use the internal or external VadjP/N DACs</t>
+  </si>
+  <si>
+    <t>LSB only, others ignored</t>
+  </si>
 </sst>
 </file>
 
@@ -1152,9 +1161,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A388" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F409" sqref="F409"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A418" sqref="A418:XFD418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12021,16 +12030,31 @@
         <v>223</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A418">
+    <row r="418" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A418" s="5">
         <v>416</v>
       </c>
-      <c r="B418" s="4" t="str">
+      <c r="B418" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A0</v>
       </c>
-      <c r="F418" t="s">
-        <v>60</v>
+      <c r="C418" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D418" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E418" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F418" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G418" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H418" s="5" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.25">
@@ -13257,7 +13281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H627"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A572" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G594" sqref="G594"/>
     </sheetView>
@@ -27031,29 +27055,29 @@
         <f t="shared" si="6"/>
         <v>01A0</v>
       </c>
-      <c r="C418">
+      <c r="C418" t="str">
         <f>'SCROD Write Registers'!C418</f>
-        <v>0</v>
-      </c>
-      <c r="D418">
+        <v>G</v>
+      </c>
+      <c r="D418" t="str">
         <f>'SCROD Write Registers'!D418</f>
-        <v>0</v>
-      </c>
-      <c r="E418">
+        <v>G</v>
+      </c>
+      <c r="E418" t="str">
         <f>'SCROD Write Registers'!E418</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F418" t="str">
         <f>'SCROD Write Registers'!F418</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G418" s="8">
+        <v>USE_EXTERNAL_VADJ_DACS</v>
+      </c>
+      <c r="G418" s="8" t="str">
         <f>'SCROD Write Registers'!G418</f>
-        <v>0</v>
-      </c>
-      <c r="H418" s="8">
+        <v>LSB chooses whether to use the internal or external VadjP/N DACs</v>
+      </c>
+      <c r="H418" s="8" t="str">
         <f>'SCROD Write Registers'!H418</f>
-        <v>0</v>
+        <v>LSB only, others ignored</v>
       </c>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Minor changes to ucf and register map.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -4,20 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="14880" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="11520" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD Write Registers" sheetId="1" r:id="rId1"/>
     <sheet name="SCROD Read Registers" sheetId="2" r:id="rId2"/>
-    <sheet name="IRS3B_TIMING_REGISTER" sheetId="4" r:id="rId3"/>
-    <sheet name="DAC Mappings (IRS2 DC RevB2)" sheetId="3" r:id="rId4"/>
+    <sheet name="IRS3B_Reg_Default" sheetId="5" r:id="rId3"/>
+    <sheet name="IRS3B_TIMING_REGISTER" sheetId="4" r:id="rId4"/>
+    <sheet name="I2C addresses" sheetId="6" r:id="rId5"/>
+    <sheet name="DAC Mappings (IRS2 DC RevB2)" sheetId="3" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">IRS3B_Reg_Default!$A$5:$K$69</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="419">
   <si>
     <t>Register Number</t>
   </si>
@@ -740,6 +745,540 @@
   </si>
   <si>
     <t>32-bit unsigned (with above)</t>
+  </si>
+  <si>
+    <t>Pulse Trigger test circuit</t>
+  </si>
+  <si>
+    <t>ADDR_M</t>
+  </si>
+  <si>
+    <t>AddrMode</t>
+  </si>
+  <si>
+    <t>Trig_In</t>
+  </si>
+  <si>
+    <t>Stop/Clear Wilkinson Reference counter</t>
+  </si>
+  <si>
+    <t>Boin_CLR</t>
+  </si>
+  <si>
+    <t>Start Wilkinson Reference counter</t>
+  </si>
+  <si>
+    <t>Start_WilkMon</t>
+  </si>
+  <si>
+    <t>Clear Read Address Registers</t>
+  </si>
+  <si>
+    <t>RD_ctr_CLR</t>
+  </si>
+  <si>
+    <t>Clear Data Output Address Registers</t>
+  </si>
+  <si>
+    <t>DatOut_ctr_CLR</t>
+  </si>
+  <si>
+    <t>undef.</t>
+  </si>
+  <si>
+    <t>0xAD0</t>
+  </si>
+  <si>
+    <t>Servo-lock target value</t>
+  </si>
+  <si>
+    <t>Timing Generator delay adjust NMOS</t>
+  </si>
+  <si>
+    <t>VadjN</t>
+  </si>
+  <si>
+    <t>0x600</t>
+  </si>
+  <si>
+    <t>DAC buff bias for VadjN</t>
+  </si>
+  <si>
+    <t>VANDbias</t>
+  </si>
+  <si>
+    <t>0x5E8</t>
+  </si>
+  <si>
+    <t>Initial config required</t>
+  </si>
+  <si>
+    <t>Timing Generator delay adjust PMOS</t>
+  </si>
+  <si>
+    <t>VadjP</t>
+  </si>
+  <si>
+    <t>DAC buff bias for VadjP</t>
+  </si>
+  <si>
+    <t>VAPDbias</t>
+  </si>
+  <si>
+    <t>0xB54</t>
+  </si>
+  <si>
+    <t>Wilkinson counter adj voltage</t>
+  </si>
+  <si>
+    <t>Vdly</t>
+  </si>
+  <si>
+    <t>0x400</t>
+  </si>
+  <si>
+    <t>DAC buff bias for Vdly</t>
+  </si>
+  <si>
+    <t>VDDbias</t>
+  </si>
+  <si>
+    <t>0x900</t>
+  </si>
+  <si>
+    <t>Voltage Ramp Current</t>
+  </si>
+  <si>
+    <t>DAC buff bias for ISEL</t>
+  </si>
+  <si>
+    <t>ISDbias</t>
+  </si>
+  <si>
+    <t>Super Buffer bias</t>
+  </si>
+  <si>
+    <t>Sbbias</t>
+  </si>
+  <si>
+    <t>DAC buff bias for Super Buffer bias</t>
+  </si>
+  <si>
+    <t>SBDbias</t>
+  </si>
+  <si>
+    <t>0xBF0</t>
+  </si>
+  <si>
+    <t>Storage Column Comparators (Pull-Up) bias</t>
+  </si>
+  <si>
+    <t>PUbias</t>
+  </si>
+  <si>
+    <t>DAC buff bias for CMPbias</t>
+  </si>
+  <si>
+    <t>PUDbias</t>
+  </si>
+  <si>
+    <t>0x500</t>
+  </si>
+  <si>
+    <t>Storage Cell Comparators (Pull-Down) bias</t>
+  </si>
+  <si>
+    <t>CMPbias</t>
+  </si>
+  <si>
+    <t>PDDbias</t>
+  </si>
+  <si>
+    <t>decode for view state --See MONTIMING Page below</t>
+  </si>
+  <si>
+    <t>Select Timing signals viewed, Phase clear, RCO running</t>
+  </si>
+  <si>
+    <t>0x***</t>
+  </si>
+  <si>
+    <t>Timing Generator Reg</t>
+  </si>
+  <si>
+    <t>0x070</t>
+  </si>
+  <si>
+    <t>Trailing Edge WR_STRB</t>
+  </si>
+  <si>
+    <t>0x040</t>
+  </si>
+  <si>
+    <t>NOTE:  WR_ADDR phase CRITICAL</t>
+  </si>
+  <si>
+    <t>Timing Gen:  WR_STRB</t>
+  </si>
+  <si>
+    <t>Leading Edge WR_STRB</t>
+  </si>
+  <si>
+    <t>0x030</t>
+  </si>
+  <si>
+    <t>Trailing Edge PHASE</t>
+  </si>
+  <si>
+    <t>0x018</t>
+  </si>
+  <si>
+    <t>Timing Gen:  PHASE</t>
+  </si>
+  <si>
+    <t>Leading Edge PHASE</t>
+  </si>
+  <si>
+    <t>Trailing Edge S2</t>
+  </si>
+  <si>
+    <t>0x068</t>
+  </si>
+  <si>
+    <t>Timing Gen:  S2</t>
+  </si>
+  <si>
+    <t>Leading Edge S2</t>
+  </si>
+  <si>
+    <t>0x058</t>
+  </si>
+  <si>
+    <t>Trailing Edge S1</t>
+  </si>
+  <si>
+    <t>0x028</t>
+  </si>
+  <si>
+    <t>Timing Gen:  S1</t>
+  </si>
+  <si>
+    <t>Leading Edge S1</t>
+  </si>
+  <si>
+    <t>0x010</t>
+  </si>
+  <si>
+    <t>Trailing Edge SSPin</t>
+  </si>
+  <si>
+    <t>0x060</t>
+  </si>
+  <si>
+    <t>Timing Gen:  SSPin</t>
+  </si>
+  <si>
+    <t>Leading Edge SSPin</t>
+  </si>
+  <si>
+    <t>0x800</t>
+  </si>
+  <si>
+    <t>Trigger threshold for reference channel</t>
+  </si>
+  <si>
+    <t>TRGthref</t>
+  </si>
+  <si>
+    <t>0x350</t>
+  </si>
+  <si>
+    <t>TRGbias for reference channel</t>
+  </si>
+  <si>
+    <t>TRGbias2</t>
+  </si>
+  <si>
+    <t>DAC buff bias for TRGbias2, TRGthref</t>
+  </si>
+  <si>
+    <t>TRGDbias</t>
+  </si>
+  <si>
+    <t>(disable for external drive)</t>
+  </si>
+  <si>
+    <t>Internal Trigger Threshold buffer bias</t>
+  </si>
+  <si>
+    <t>Tbbias</t>
+  </si>
+  <si>
+    <t>DAC buff bias for Trigger Thresholds</t>
+  </si>
+  <si>
+    <t>THDbias</t>
+  </si>
+  <si>
+    <t>Trigger Comparator bias</t>
+  </si>
+  <si>
+    <t>TRGbias</t>
+  </si>
+  <si>
+    <t>DAC buff bias for Trigger Comparator</t>
+  </si>
+  <si>
+    <t>TCBbias</t>
+  </si>
+  <si>
+    <t>0x370</t>
+  </si>
+  <si>
+    <t>Trigger Width adjust (Wbias)</t>
+  </si>
+  <si>
+    <t>0x3D7</t>
+  </si>
+  <si>
+    <t>Wbias</t>
+  </si>
+  <si>
+    <t>DAC buff bias for Wbias</t>
+  </si>
+  <si>
+    <t>WBDbias</t>
+  </si>
+  <si>
+    <t>0x000</t>
+  </si>
+  <si>
+    <t>Misc Reg (incl. SGN)</t>
+  </si>
+  <si>
+    <t>Buff amp bias -- transfer samples</t>
+  </si>
+  <si>
+    <t>Vbias2</t>
+  </si>
+  <si>
+    <t>0x380</t>
+  </si>
+  <si>
+    <t>Buff amp bias -- initial sample</t>
+  </si>
+  <si>
+    <t>Vbias</t>
+  </si>
+  <si>
+    <t>DAC buff bias for Vbias, Vbias2</t>
+  </si>
+  <si>
+    <t>VBDbias</t>
+  </si>
+  <si>
+    <t>TBD (0x000)</t>
+  </si>
+  <si>
+    <t>Threshold Ch. 8</t>
+  </si>
+  <si>
+    <t>Threshold Ch. 7</t>
+  </si>
+  <si>
+    <t>Threshold Ch. 6</t>
+  </si>
+  <si>
+    <t>Threshold Ch. 5</t>
+  </si>
+  <si>
+    <t>Threshold Ch. 4</t>
+  </si>
+  <si>
+    <t>Threshold Ch. 3</t>
+  </si>
+  <si>
+    <t>Threshold Ch. 2</t>
+  </si>
+  <si>
+    <t>scan required</t>
+  </si>
+  <si>
+    <t>Threshold Ch. 1</t>
+  </si>
+  <si>
+    <t>equiv.</t>
+  </si>
+  <si>
+    <t>value (hex)</t>
+  </si>
+  <si>
+    <t># bits</t>
+  </si>
+  <si>
+    <t>Default value</t>
+  </si>
+  <si>
+    <t>Register/Value</t>
+  </si>
+  <si>
+    <t>"PCLK #"</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>mV/count</t>
+  </si>
+  <si>
+    <t>Decimal equivalent at right --&gt;</t>
+  </si>
+  <si>
+    <t>counts</t>
+  </si>
+  <si>
+    <t>mV</t>
+  </si>
+  <si>
+    <t>Register Map for IRS3B</t>
+  </si>
+  <si>
+    <t>alternative is to treat GPIO2 on c13 as write-only device and ignore the conflict with the temperature sensor (which it will not be possible to read)</t>
+  </si>
+  <si>
+    <t>the boxes with a red background are a mistake; solution is to exchange for PCA9534, then the address is 0100010</t>
+  </si>
+  <si>
+    <t>swapped GPIO0 and GPIO2 in this table from previous version to make it correspond to the schematic</t>
+  </si>
+  <si>
+    <t>updates from 2013-03-01:</t>
+  </si>
+  <si>
+    <t>W18,J2</t>
+  </si>
+  <si>
+    <t>GPIOs are PCA9534</t>
+  </si>
+  <si>
+    <t>interconnect</t>
+  </si>
+  <si>
+    <t>0100001</t>
+  </si>
+  <si>
+    <t>0100000</t>
+  </si>
+  <si>
+    <t>0111011</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>0111010</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1001011</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0010001</t>
+  </si>
+  <si>
+    <t>0111000</t>
+  </si>
+  <si>
+    <t>0111001</t>
+  </si>
+  <si>
+    <t>1010001</t>
+  </si>
+  <si>
+    <t>1001010</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1001001</t>
+  </si>
+  <si>
+    <t>0010000</t>
+  </si>
+  <si>
+    <t>0111100</t>
+  </si>
+  <si>
+    <t>0111101</t>
+  </si>
+  <si>
+    <t>0111110</t>
+  </si>
+  <si>
+    <t>1010000</t>
+  </si>
+  <si>
+    <t>1001000</t>
+  </si>
+  <si>
+    <t>I2C SCL,SDA nets</t>
+  </si>
+  <si>
+    <t>E14,K14</t>
+  </si>
+  <si>
+    <t>AB4,P19</t>
+  </si>
+  <si>
+    <t>L10,K10</t>
+  </si>
+  <si>
+    <t>GPIOs are PCA9534A</t>
+  </si>
+  <si>
+    <t>H13,F14</t>
+  </si>
+  <si>
+    <t>AD4,AE1</t>
+  </si>
+  <si>
+    <t>M18,N18</t>
+  </si>
+  <si>
+    <t>carrier DAC</t>
+  </si>
+  <si>
+    <t>carrier GPIO0</t>
+  </si>
+  <si>
+    <t>carrier GPIO1</t>
+  </si>
+  <si>
+    <t>carrier GPIO2</t>
+  </si>
+  <si>
+    <t>carrier eeprom</t>
+  </si>
+  <si>
+    <t>ASIC temperature</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>row</t>
   </si>
 </sst>
 </file>
@@ -749,7 +1288,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,8 +1304,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -777,6 +1344,48 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="25"/>
+        <bgColor indexed="61"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="60"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="49"/>
+        <bgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+        <bgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
+        <bgColor indexed="15"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor indexed="35"/>
       </patternFill>
     </fill>
   </fills>
@@ -807,10 +1416,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -855,9 +1465,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1158,9 +1837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A497" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G504" sqref="G504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13122,9 +13801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H628"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A601" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F610" sqref="F610"/>
+      <selection pane="bottomLeft" activeCell="A610" sqref="A610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32737,10 +33416,1608 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q69"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E1" s="31">
+        <f ca="1">+TODAY()</f>
+        <v>41349</v>
+      </c>
+      <c r="P1">
+        <v>2500</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E2" s="31"/>
+      <c r="P2">
+        <v>4096</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E3" s="31"/>
+      <c r="P3">
+        <f>+P1/P2</f>
+        <v>0.6103515625</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N4" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D5" t="s">
+        <v>363</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
+        <v>1</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="D6" s="28">
+        <v>12</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>HEX2DEC(N6)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="25">
+        <f>+$P$3*O6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="28">
+        <v>2</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="D7" s="28">
+        <v>12</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>HEX2DEC(N7)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="25">
+        <f>+$P$3*O7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
+        <v>3</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="D8" s="28">
+        <v>12</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>HEX2DEC(N8)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="25">
+        <f>+$P$3*O8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>4</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>356</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="D9" s="28">
+        <v>12</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>HEX2DEC(N9)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="25">
+        <f>+$P$3*O9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="28">
+        <v>5</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="D10" s="28">
+        <v>12</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>HEX2DEC(N10)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="25">
+        <f>+$P$3*O10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="28">
+        <v>6</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="D11" s="28">
+        <v>12</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>HEX2DEC(N11)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="25">
+        <f>+$P$3*O11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="28">
+        <v>7</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="D12" s="28">
+        <v>12</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>HEX2DEC(N12)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="25">
+        <f>+$P$3*O12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26">
+        <v>8</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="D13" s="26">
+        <v>12</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>HEX2DEC(N13)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="25">
+        <f>+$P$3*O13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>350</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>349</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="N14" s="24">
+        <v>400</v>
+      </c>
+      <c r="O14">
+        <f>HEX2DEC(N14)</f>
+        <v>1024</v>
+      </c>
+      <c r="P14" s="25">
+        <f>+$P$3*O14</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>348</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>347</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="N15" s="24">
+        <v>380</v>
+      </c>
+      <c r="O15">
+        <f>HEX2DEC(N15)</f>
+        <v>896</v>
+      </c>
+      <c r="P15" s="25">
+        <f>+$P$3*O15</f>
+        <v>546.875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>345</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>344</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="N16" s="24">
+        <v>370</v>
+      </c>
+      <c r="O16">
+        <f>HEX2DEC(N16)</f>
+        <v>880</v>
+      </c>
+      <c r="P16" s="25">
+        <f>+$P$3*O16</f>
+        <v>537.109375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>343</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="N17" s="24">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>HEX2DEC(N17)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="25">
+        <f>+$P$3*O17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>341</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>340</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="N18" s="24">
+        <v>400</v>
+      </c>
+      <c r="O18">
+        <f>HEX2DEC(N18)</f>
+        <v>1024</v>
+      </c>
+      <c r="P18" s="25">
+        <f>+$P$3*O18</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>339</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>337</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="N19" s="24">
+        <v>370</v>
+      </c>
+      <c r="O19">
+        <f>HEX2DEC(N19)</f>
+        <v>880</v>
+      </c>
+      <c r="P19" s="25">
+        <f>+$P$3*O19</f>
+        <v>537.109375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>335</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>334</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="N20" s="24">
+        <v>400</v>
+      </c>
+      <c r="O20">
+        <f>HEX2DEC(N20)</f>
+        <v>1024</v>
+      </c>
+      <c r="P20" s="25">
+        <f>+$P$3*O20</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>333</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>332</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="N21" s="24">
+        <v>350</v>
+      </c>
+      <c r="O21">
+        <f>HEX2DEC(N21)</f>
+        <v>848</v>
+      </c>
+      <c r="P21" s="25">
+        <f>+$P$3*O21</f>
+        <v>517.578125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>331</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>330</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="N22" s="24">
+        <v>400</v>
+      </c>
+      <c r="O22">
+        <f>HEX2DEC(N22)</f>
+        <v>1024</v>
+      </c>
+      <c r="P22" s="25">
+        <f>+$P$3*O22</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>329</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>328</v>
+      </c>
+      <c r="I23" t="s">
+        <v>327</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="N23" s="24">
+        <v>400</v>
+      </c>
+      <c r="O23">
+        <f>HEX2DEC(N23)</f>
+        <v>1024</v>
+      </c>
+      <c r="P23" s="25">
+        <f>+$P$3*O23</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>326</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>325</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="N24" s="24">
+        <v>400</v>
+      </c>
+      <c r="O24">
+        <f>HEX2DEC(N24)</f>
+        <v>1024</v>
+      </c>
+      <c r="P24" s="25">
+        <f>+$P$3*O24</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>324</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>323</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="N25" s="24">
+        <v>350</v>
+      </c>
+      <c r="O25">
+        <f>HEX2DEC(N25)</f>
+        <v>848</v>
+      </c>
+      <c r="P25" s="25">
+        <f>+$P$3*O25</f>
+        <v>517.578125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>321</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>320</v>
+      </c>
+      <c r="M26" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="N26" s="24">
+        <v>800</v>
+      </c>
+      <c r="O26">
+        <f>HEX2DEC(N26)</f>
+        <v>2048</v>
+      </c>
+      <c r="P26" s="25">
+        <f>+$P$3*O26</f>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="M27" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="N27" s="24">
+        <v>60</v>
+      </c>
+      <c r="O27">
+        <f>HEX2DEC(N27)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>+A27+1</f>
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>315</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="M28" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="N28" s="24">
+        <v>10</v>
+      </c>
+      <c r="O28">
+        <f>HEX2DEC(N28)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f>+A28+1</f>
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>313</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="M29" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="N29" s="24">
+        <v>28</v>
+      </c>
+      <c r="O29">
+        <f>HEX2DEC(N29)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>+A29+1</f>
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>310</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="M30" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="N30" s="24">
+        <v>58</v>
+      </c>
+      <c r="O30">
+        <f>HEX2DEC(N30)</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>+A30+1</f>
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>308</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="M31" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="N31" s="24">
+        <v>68</v>
+      </c>
+      <c r="O31">
+        <f>HEX2DEC(N31)</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>+A31+1</f>
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>305</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="M32" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="N32" s="24">
+        <v>18</v>
+      </c>
+      <c r="O32">
+        <f>HEX2DEC(N32)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>+A32+1</f>
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>304</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="M33" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="N33" s="24">
+        <v>18</v>
+      </c>
+      <c r="O33">
+        <f>HEX2DEC(N33)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f>+A33+1</f>
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>301</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="M34" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="N34" s="24">
+        <v>30</v>
+      </c>
+      <c r="O34">
+        <f>HEX2DEC(N34)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f>+A34+1</f>
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="N35" s="24">
+        <v>40</v>
+      </c>
+      <c r="O35">
+        <f>HEX2DEC(N35)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>+A35+1</f>
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>295</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="M36" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="N36" s="24">
+        <v>70</v>
+      </c>
+      <c r="O36">
+        <f>HEX2DEC(N36)</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>+A36+1</f>
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>293</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>291</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>+A37+1</f>
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>289</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D38">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>284</v>
+      </c>
+      <c r="M38" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>+A38+1</f>
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>288</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="D39">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>287</v>
+      </c>
+      <c r="M39" s="15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>+A39+1</f>
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>285</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D40">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
+        <v>284</v>
+      </c>
+      <c r="M40" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>+A40+1</f>
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>283</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="D41">
+        <v>12</v>
+      </c>
+      <c r="E41" t="s">
+        <v>282</v>
+      </c>
+      <c r="M41" s="15" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f>+A41+1</f>
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>280</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s">
+        <v>279</v>
+      </c>
+      <c r="M42" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f>+A42+1</f>
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>278</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D43">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
+        <v>277</v>
+      </c>
+      <c r="M43" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f>+A43+1</f>
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>276</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D44">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>275</v>
+      </c>
+      <c r="M44" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f>+A44+1</f>
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="D45">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>274</v>
+      </c>
+      <c r="I45" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="M45" s="15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f>+A45+1</f>
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>272</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D46">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>271</v>
+      </c>
+      <c r="M46" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f>+A46+1</f>
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="D47">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
+        <v>268</v>
+      </c>
+      <c r="I47" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="M47" s="15" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f>+A47+1</f>
+        <v>43</v>
+      </c>
+      <c r="B48" t="s">
+        <v>266</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48">
+        <v>12</v>
+      </c>
+      <c r="E48" t="s">
+        <v>265</v>
+      </c>
+      <c r="M48" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f>+A48+1</f>
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>264</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="D49">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
+        <v>263</v>
+      </c>
+      <c r="I49" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="M49" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f>+A49+1</f>
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>260</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50">
+        <v>12</v>
+      </c>
+      <c r="E50" t="s">
+        <v>259</v>
+      </c>
+      <c r="M50" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f>+A50+1</f>
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>257</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="D51">
+        <v>12</v>
+      </c>
+      <c r="E51" t="s">
+        <v>256</v>
+      </c>
+      <c r="I51" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="M51" s="15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f>+A51+1</f>
+        <v>47</v>
+      </c>
+      <c r="C52" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f>+A52+1</f>
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f>+A53+1</f>
+        <v>49</v>
+      </c>
+      <c r="C54" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f>+A54+1</f>
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f>+A55+1</f>
+        <v>51</v>
+      </c>
+      <c r="C56" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f>+A56+1</f>
+        <v>52</v>
+      </c>
+      <c r="C57" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f>+A57+1</f>
+        <v>53</v>
+      </c>
+      <c r="C58" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f>+A58+1</f>
+        <v>54</v>
+      </c>
+      <c r="C59" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f>+A59+1</f>
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f>+A60+1</f>
+        <v>56</v>
+      </c>
+      <c r="C61" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f>+A61+1</f>
+        <v>57</v>
+      </c>
+      <c r="C62" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f>+A62+1</f>
+        <v>58</v>
+      </c>
+      <c r="C63" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f>+A63+1</f>
+        <v>59</v>
+      </c>
+      <c r="C64" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f>+A64+1</f>
+        <v>60</v>
+      </c>
+      <c r="B65" t="s">
+        <v>252</v>
+      </c>
+      <c r="C65" t="s">
+        <v>243</v>
+      </c>
+      <c r="D65" t="s">
+        <v>242</v>
+      </c>
+      <c r="E65" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f>+A65+1</f>
+        <v>61</v>
+      </c>
+      <c r="B66" t="s">
+        <v>250</v>
+      </c>
+      <c r="C66" t="s">
+        <v>243</v>
+      </c>
+      <c r="D66" t="s">
+        <v>242</v>
+      </c>
+      <c r="E66" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f>+A66+1</f>
+        <v>62</v>
+      </c>
+      <c r="B67" t="s">
+        <v>248</v>
+      </c>
+      <c r="C67" t="s">
+        <v>243</v>
+      </c>
+      <c r="D67" t="s">
+        <v>242</v>
+      </c>
+      <c r="E67" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f>+A67+1</f>
+        <v>63</v>
+      </c>
+      <c r="B68" t="s">
+        <v>246</v>
+      </c>
+      <c r="C68" t="s">
+        <v>243</v>
+      </c>
+      <c r="D68" t="s">
+        <v>242</v>
+      </c>
+      <c r="E68" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f>+A68+1</f>
+        <v>64</v>
+      </c>
+      <c r="B69" t="s">
+        <v>244</v>
+      </c>
+      <c r="C69" t="s">
+        <v>243</v>
+      </c>
+      <c r="D69" t="s">
+        <v>242</v>
+      </c>
+      <c r="E69" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E35:G36"/>
+    <mergeCell ref="E6:E13"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="E29:F30"/>
+    <mergeCell ref="E31:F32"/>
+    <mergeCell ref="E33:F34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="72" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32979,13 +35256,549 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="32" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="32" customWidth="1"/>
+    <col min="5" max="7" width="12.7109375" style="32" customWidth="1"/>
+    <col min="8" max="8" width="11" style="32" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="33" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" style="33" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="33" customWidth="1"/>
+    <col min="12" max="12" width="11" style="33" customWidth="1"/>
+    <col min="13" max="16384" width="11.5703125" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>418</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>416</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>415</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>414</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>412</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C2" s="44" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="46" t="s">
+        <v>409</v>
+      </c>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47" t="s">
+        <v>408</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>402</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>401</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>400</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>399</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>398</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>396</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="43"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>391</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="43"/>
+      <c r="J5" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="43"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>394</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>393</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="F7" s="46" t="s">
+        <v>392</v>
+      </c>
+      <c r="G7" s="46" t="s">
+        <v>391</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>390</v>
+      </c>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>388</v>
+      </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="43"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>386</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="43"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>384</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="43"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="39" t="s">
+        <v>406</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="41" t="s">
+        <v>405</v>
+      </c>
+      <c r="G11" s="41"/>
+      <c r="H11" s="42" t="s">
+        <v>404</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>402</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>400</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>399</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>398</v>
+      </c>
+      <c r="H12" s="37" t="s">
+        <v>397</v>
+      </c>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="37"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>391</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="37"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>392</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="37"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>394</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>393</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>392</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>391</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>390</v>
+      </c>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>388</v>
+      </c>
+      <c r="D17" s="39"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="37"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>386</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="37"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>384</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="37"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="35"/>
+      <c r="E21" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>381</v>
+      </c>
+      <c r="J21" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="K21" s="35" t="s">
+        <v>379</v>
+      </c>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C23" s="36" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C24" s="35" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="34" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="34" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C27" s="34"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="24">
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="G3:G6"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added the following features: monitor header pins now let you monitor RCOSSX and MONTIMING, with ASIC selectable by register 380.  Counter has been added to read register 610 that reports the number of seconds since the SST PLL was not locked.  Register map updated.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="11520" windowHeight="7965"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="11520" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD Write Registers" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="425">
   <si>
     <t>Register Number</t>
   </si>
@@ -1279,6 +1279,24 @@
   </si>
   <si>
     <t>Bits 7:0 timing reg (ASIC register), Bit 8: Signal for the sampling block to perform the sync  - set to one after all taps/biases are programmed, Bits 10:9 Choose which phase to use among 4 PHAB phases</t>
+  </si>
+  <si>
+    <t>Seconds SST PLL locked</t>
+  </si>
+  <si>
+    <t>Number of seconds the PLL generating SST_IN has been locked</t>
+  </si>
+  <si>
+    <t>16-bit unsigned</t>
+  </si>
+  <si>
+    <t>Choose which MONTIMING and RCOSSX signal to send to the monitor headers</t>
+  </si>
+  <si>
+    <t>Bits 1:0 row MONTIMING, bits 3:2 col MONTIMING, bits 5:4 row RCOSSX, bits 7:6 col RCOSSX</t>
+  </si>
+  <si>
+    <t>MON_HEADER_MON_TIMING_ROW/COL (&amp; RCOSSX)</t>
   </si>
 </sst>
 </file>
@@ -1837,16 +1855,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G381" sqref="G381"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B382" sqref="B382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="108" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11638,16 +11656,31 @@
         <v>418</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A382">
+    <row r="382" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A382" s="5">
         <v>380</v>
       </c>
-      <c r="B382" s="4" t="str">
+      <c r="B382" s="7" t="str">
         <f t="shared" si="6"/>
         <v>017C</v>
       </c>
-      <c r="F382" t="s">
-        <v>60</v>
+      <c r="C382" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D382" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E382" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F382" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="G382" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="H382" s="5" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -13801,9 +13834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H628"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G600" sqref="G600"/>
+      <selection pane="bottomLeft" activeCell="G603" sqref="G603"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26387,29 +26420,29 @@
         <f t="shared" si="5"/>
         <v>017C</v>
       </c>
-      <c r="C382">
+      <c r="C382" t="str">
         <f>'SCROD Write Registers'!C382</f>
-        <v>0</v>
-      </c>
-      <c r="D382">
+        <v>N/A</v>
+      </c>
+      <c r="D382" t="str">
         <f>'SCROD Write Registers'!D382</f>
-        <v>0</v>
-      </c>
-      <c r="E382">
+        <v>N/A</v>
+      </c>
+      <c r="E382" t="str">
         <f>'SCROD Write Registers'!E382</f>
-        <v>0</v>
+        <v>N/A</v>
       </c>
       <c r="F382" t="str">
         <f>'SCROD Write Registers'!F382</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G382" s="8">
+        <v>MON_HEADER_MON_TIMING_ROW/COL (&amp; RCOSSX)</v>
+      </c>
+      <c r="G382" s="8" t="str">
         <f>'SCROD Write Registers'!G382</f>
-        <v>0</v>
-      </c>
-      <c r="H382" s="8">
+        <v>Choose which MONTIMING and RCOSSX signal to send to the monitor headers</v>
+      </c>
+      <c r="H382" s="8" t="str">
         <f>'SCROD Write Registers'!H382</f>
-        <v>0</v>
+        <v>Bits 1:0 row MONTIMING, bits 3:2 col MONTIMING, bits 5:4 row RCOSSX, bits 7:6 col RCOSSX</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -32606,7 +32639,7 @@
         <v>582</v>
       </c>
       <c r="B584" s="6" t="str">
-        <f t="shared" ref="B584:B611" si="11">DEC2HEX(A584,4)</f>
+        <f t="shared" ref="B584:B612" si="11">DEC2HEX(A584,4)</f>
         <v>0246</v>
       </c>
       <c r="C584" s="5">
@@ -33357,8 +33390,32 @@
         <v>238</v>
       </c>
     </row>
-    <row r="612" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B612" s="3"/>
+    <row r="612" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A612" s="5">
+        <v>610</v>
+      </c>
+      <c r="B612" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>0262</v>
+      </c>
+      <c r="C612" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D612" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E612" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F612" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G612" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="H612" s="5" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="613" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B613" s="3"/>
@@ -35017,7 +35074,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Quick changes to incorporate new monitoring signals.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="11520" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="11520" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD Write Registers" sheetId="1" r:id="rId1"/>
@@ -1293,10 +1293,10 @@
     <t>Choose which MONTIMING and RCOSSX signal to send to the monitor headers</t>
   </si>
   <si>
-    <t>Bits 1:0 row MONTIMING, bits 3:2 col MONTIMING, bits 5:4 row RCOSSX, bits 7:6 col RCOSSX</t>
-  </si>
-  <si>
     <t>MON_HEADER_MON_TIMING_ROW/COL (&amp; RCOSSX)</t>
+  </si>
+  <si>
+    <t>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 5: choose between MONTIMING and RCOSSX</t>
   </si>
 </sst>
 </file>
@@ -1855,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B382" sqref="B382"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H383" sqref="H383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11674,13 +11674,13 @@
         <v>10</v>
       </c>
       <c r="F382" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G382" s="5" t="s">
         <v>422</v>
       </c>
       <c r="H382" s="5" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -13834,8 +13834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H628"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A557" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G603" sqref="G603"/>
     </sheetView>
   </sheetViews>
@@ -26442,7 +26442,7 @@
       </c>
       <c r="H382" s="8" t="str">
         <f>'SCROD Write Registers'!H382</f>
-        <v>Bits 1:0 row MONTIMING, bits 3:2 col MONTIMING, bits 5:4 row RCOSSX, bits 7:6 col RCOSSX</v>
+        <v>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 5: choose between MONTIMING and RCOSSX</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -33478,8 +33478,8 @@
   </sheetPr>
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Re-added location constraint for FTSW PLL.  Added some monitoring to debug sampling state machine.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -1275,9 +1275,6 @@
     <t>row</t>
   </si>
   <si>
-    <t>TIMING_REG &amp; sampling sync bits)</t>
-  </si>
-  <si>
     <t>Bits 7:0 timing reg (ASIC register), Bit 8: Signal for the sampling block to perform the sync  - set to one after all taps/biases are programmed, Bits 10:9 Choose which phase to use among 4 PHAB phases</t>
   </si>
   <si>
@@ -1297,6 +1294,9 @@
   </si>
   <si>
     <t>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 5: choose between MONTIMING and RCOSSX</t>
+  </si>
+  <si>
+    <t>TIMING_REG &amp; sampling sync bits</t>
   </si>
 </sst>
 </file>
@@ -1855,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H383" sqref="H383"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A381" sqref="A381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11647,13 +11647,13 @@
         <v>5</v>
       </c>
       <c r="F381" s="5" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="G381" s="5" t="s">
         <v>200</v>
       </c>
       <c r="H381" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="382" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -11674,13 +11674,13 @@
         <v>10</v>
       </c>
       <c r="F382" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G382" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="H382" s="5" t="s">
         <v>423</v>
-      </c>
-      <c r="G382" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="H382" s="5" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -13835,7 +13835,7 @@
   <dimension ref="A1:H628"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A557" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A596" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G603" sqref="G603"/>
     </sheetView>
   </sheetViews>
@@ -26401,7 +26401,7 @@
       </c>
       <c r="F381" t="str">
         <f>'SCROD Write Registers'!F381</f>
-        <v>TIMING_REG &amp; sampling sync bits)</v>
+        <v>TIMING_REG &amp; sampling sync bits</v>
       </c>
       <c r="G381" s="8" t="str">
         <f>'SCROD Write Registers'!G381</f>
@@ -33408,13 +33408,13 @@
         <v>10</v>
       </c>
       <c r="F612" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G612" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="G612" s="5" t="s">
+      <c r="H612" s="5" t="s">
         <v>420</v>
-      </c>
-      <c r="H612" s="5" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="613" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commited changes to chipscope project to monitor SDR section, including checking state of sampling block.  Found a dangling signal to sampling block.  now the same MONTIMING signal that is selected for the monitor header is used to drive the alignment in the sampling block.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -1293,10 +1293,10 @@
     <t>MON_HEADER_MON_TIMING_ROW/COL (&amp; RCOSSX)</t>
   </si>
   <si>
-    <t>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 5: choose between MONTIMING and RCOSSX</t>
-  </si>
-  <si>
     <t>TIMING_REG &amp; sampling sync bits</t>
+  </si>
+  <si>
+    <t>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 4: choose between MONTIMING and RCOSSX</t>
   </si>
 </sst>
 </file>
@@ -1855,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A381" sqref="A381"/>
+      <selection pane="bottomLeft" activeCell="H383" sqref="H383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11647,7 +11647,7 @@
         <v>5</v>
       </c>
       <c r="F381" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G381" s="5" t="s">
         <v>200</v>
@@ -11680,7 +11680,7 @@
         <v>421</v>
       </c>
       <c r="H382" s="5" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -26442,7 +26442,7 @@
       </c>
       <c r="H382" s="8" t="str">
         <f>'SCROD Write Registers'!H382</f>
-        <v>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 5: choose between MONTIMING and RCOSSX</v>
+        <v>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 4: choose between MONTIMING and RCOSSX</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -33495,7 +33495,7 @@
       </c>
       <c r="E1" s="27">
         <f ca="1">+TODAY()</f>
-        <v>41357</v>
+        <v>41358</v>
       </c>
       <c r="P1">
         <v>2500</v>
@@ -35074,7 +35074,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commited changes to chipscope project to monitor SDR section, including checking state of sampling block.  Found a dangling signal to sampling block.  now the same MONTIMING signal that is selected for the monitor header is used to drive the alignment in the sampling block.  Fixed a typo in the register map for register 380 bit mapping.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -1855,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H383" sqref="H383"/>
+      <selection pane="bottomLeft" activeCell="A382" sqref="A382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Luca's suggested modification to the sampling block to fix the synchronization.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -1530,25 +1530,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1857,7 +1857,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A382" sqref="A382"/>
+      <selection pane="bottomLeft" activeCell="A381" sqref="A381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35363,15 +35363,15 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="41" t="s">
         <v>408</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42" t="s">
         <v>407</v>
       </c>
-      <c r="G2" s="47"/>
+      <c r="G2" s="42"/>
       <c r="H2" s="36" t="s">
         <v>406</v>
       </c>
@@ -35389,19 +35389,19 @@
       <c r="C3" s="35" t="s">
         <v>400</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="41" t="s">
         <v>399</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="41" t="s">
         <v>398</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="42" t="s">
         <v>397</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="42" t="s">
         <v>396</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="43" t="s">
         <v>395</v>
       </c>
     </row>
@@ -35415,11 +35415,11 @@
       <c r="C4" s="35" t="s">
         <v>394</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="45"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="43"/>
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
       <c r="M4" s="31"/>
@@ -35435,11 +35435,11 @@
       <c r="C5" s="35" t="s">
         <v>389</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="45"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="43"/>
       <c r="J5" s="29" t="s">
         <v>405</v>
       </c>
@@ -35458,11 +35458,11 @@
       <c r="C6" s="35" t="s">
         <v>390</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="45"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="43"/>
       <c r="K6" s="31"/>
       <c r="L6" s="31"/>
       <c r="M6" s="31"/>
@@ -35478,19 +35478,19 @@
       <c r="C7" s="35" t="s">
         <v>392</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="41" t="s">
         <v>391</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="44" t="s">
         <v>384</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="42" t="s">
         <v>390</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="G7" s="42" t="s">
         <v>389</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="43" t="s">
         <v>388</v>
       </c>
       <c r="K7" s="31"/>
@@ -35508,11 +35508,11 @@
       <c r="C8" s="35" t="s">
         <v>386</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="45"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="43"/>
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
       <c r="L8" s="31"/>
@@ -35529,11 +35529,11 @@
       <c r="C9" s="35" t="s">
         <v>384</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="45"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="43"/>
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
       <c r="L9" s="31"/>
@@ -35550,11 +35550,11 @@
       <c r="C10" s="35" t="s">
         <v>382</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="45"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="43"/>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
@@ -35562,15 +35562,15 @@
       <c r="N10" s="31"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="45" t="s">
         <v>404</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="44" t="s">
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="46"/>
       <c r="H11" s="34" t="s">
         <v>402</v>
       </c>
@@ -35592,19 +35592,19 @@
       <c r="C12" s="33" t="s">
         <v>400</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="45" t="s">
         <v>399</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="45" t="s">
         <v>398</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="G12" s="46" t="s">
         <v>396</v>
       </c>
-      <c r="H12" s="41" t="s">
+      <c r="H12" s="47" t="s">
         <v>395</v>
       </c>
       <c r="K12" s="31"/>
@@ -35622,11 +35622,11 @@
       <c r="C13" s="33" t="s">
         <v>394</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="41"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="47"/>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
       <c r="M13" s="31"/>
@@ -35642,11 +35642,11 @@
       <c r="C14" s="33" t="s">
         <v>389</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="41"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="47"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
       <c r="M14" s="31"/>
@@ -35662,11 +35662,11 @@
       <c r="C15" s="33" t="s">
         <v>390</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="41"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="47"/>
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
       <c r="M15" s="31"/>
@@ -35682,19 +35682,19 @@
       <c r="C16" s="33" t="s">
         <v>392</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="45" t="s">
         <v>391</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="44" t="s">
         <v>384</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="46" t="s">
         <v>390</v>
       </c>
-      <c r="G16" s="44" t="s">
+      <c r="G16" s="46" t="s">
         <v>389</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="47" t="s">
         <v>388</v>
       </c>
       <c r="K16" s="31"/>
@@ -35712,11 +35712,11 @@
       <c r="C17" s="33" t="s">
         <v>386</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="41"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="47"/>
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
       <c r="M17" s="31"/>
@@ -35732,11 +35732,11 @@
       <c r="C18" s="33" t="s">
         <v>384</v>
       </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="41"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="47"/>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
       <c r="M18" s="31"/>
@@ -35752,11 +35752,11 @@
       <c r="C19" s="33" t="s">
         <v>382</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="41"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="47"/>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
       <c r="M19" s="31"/>
@@ -35815,30 +35815,30 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="24">
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="G3:G6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
A number of changes have been made: CLKx4SST has been removed in favor of CLKx2SST to make the timing margins easier for the firmware to infer automatically.  The CE that was previously used divide CLKx4SST by 2 to produce effectively SSTx2 is now gone.  Timing constraints have been added, mostly ignores for false paths, so that the design now passes timing.  Fixed a bug in the channel/sample serial loading that was causing the MSB of the channel to always be loaded as a zero.  Rewrote some ROI code for clarity, and hopefully to fix a bug that was causing incorrect windows to be read out.  Trying now to handle the write/read address remappings, but this is not quite working yet...
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="11280" windowHeight="7965"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="11280" windowHeight="7965" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD Write Registers" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="441">
   <si>
     <t>Register Number</t>
   </si>
@@ -1333,6 +1333,18 @@
   </si>
   <si>
     <t>montiming output</t>
+  </si>
+  <si>
+    <t>BF0</t>
+  </si>
+  <si>
+    <t>B54</t>
+  </si>
+  <si>
+    <t>5E8</t>
+  </si>
+  <si>
+    <t>AD0</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1493,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1608,6 +1620,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -1913,9 +1927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13892,8 +13906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H628"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A596" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G603" sqref="G603"/>
     </sheetView>
   </sheetViews>
@@ -33536,8 +33550,8 @@
   </sheetPr>
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33646,7 +33660,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O36" si="0">HEX2DEC(N6)</f>
+        <f t="shared" ref="O6:O51" si="0">HEX2DEC(N6)</f>
         <v>0</v>
       </c>
       <c r="P6" s="22">
@@ -34620,6 +34634,13 @@
       <c r="M38" s="14" t="s">
         <v>257</v>
       </c>
+      <c r="N38">
+        <v>400</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -34641,6 +34662,13 @@
       <c r="M39" s="14" t="s">
         <v>273</v>
       </c>
+      <c r="N39">
+        <v>500</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="0"/>
+        <v>1280</v>
+      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -34662,6 +34690,13 @@
       <c r="M40" s="14" t="s">
         <v>257</v>
       </c>
+      <c r="N40">
+        <v>400</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -34683,6 +34718,13 @@
       <c r="M41" s="14" t="s">
         <v>268</v>
       </c>
+      <c r="N41" t="s">
+        <v>437</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="0"/>
+        <v>3056</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -34704,6 +34746,13 @@
       <c r="M42" s="14" t="s">
         <v>257</v>
       </c>
+      <c r="N42">
+        <v>400</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -34725,6 +34774,13 @@
       <c r="M43" s="14" t="s">
         <v>257</v>
       </c>
+      <c r="N43">
+        <v>400</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -34746,6 +34802,13 @@
       <c r="M44" s="14" t="s">
         <v>257</v>
       </c>
+      <c r="N44">
+        <v>400</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -34770,6 +34833,13 @@
       <c r="M45" s="14" t="s">
         <v>260</v>
       </c>
+      <c r="N45">
+        <v>900</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="0"/>
+        <v>2304</v>
+      </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -34791,6 +34861,13 @@
       <c r="M46" s="14" t="s">
         <v>257</v>
       </c>
+      <c r="N46">
+        <v>400</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -34815,6 +34892,13 @@
       <c r="M47" s="14" t="s">
         <v>254</v>
       </c>
+      <c r="N47" t="s">
+        <v>438</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -34836,8 +34920,15 @@
       <c r="M48" s="14" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <v>600</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="0"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -34860,8 +34951,15 @@
       <c r="M49" s="14" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49" s="54" t="s">
+        <v>439</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="0"/>
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -34881,8 +34979,15 @@
       <c r="M50" s="14" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <v>600</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="0"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -34905,8 +35010,15 @@
       <c r="M51" s="14" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51" s="55" t="s">
+        <v>440</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="0"/>
+        <v>2768</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -34915,7 +35027,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -34924,7 +35036,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -34933,7 +35045,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -34942,7 +35054,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -34951,7 +35063,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -34960,7 +35072,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="2"/>
         <v>53</v>
@@ -34969,7 +35081,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="2"/>
         <v>54</v>
@@ -34978,7 +35090,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -34987,7 +35099,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="2"/>
         <v>56</v>
@@ -34996,7 +35108,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -35005,7 +35117,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -35014,7 +35126,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="2"/>
         <v>59</v>

</xml_diff>

<commit_message>
Added an extra bit to register 379 to allow toggling between the two possibilities for the LSB of the write address.  Added a read register at 611 for firmware revision.  This is controlled by a small package definition at the top of scrod_top.vhd.  This should now be updated before any commit.  Updated register map to reflect these two changes.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="11280" windowHeight="7965"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="11280" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD Write Registers" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="443">
   <si>
     <t>Register Number</t>
   </si>
@@ -1239,9 +1239,6 @@
     <t>row</t>
   </si>
   <si>
-    <t>Bits 7:0 timing reg (ASIC register), Bit 8: Signal for the sampling block to perform the sync  - set to one after all taps/biases are programmed, Bits 10:9 Choose which phase to use among 4 PHAB phases</t>
-  </si>
-  <si>
     <t>Seconds SST PLL locked</t>
   </si>
   <si>
@@ -1345,6 +1342,15 @@
   </si>
   <si>
     <t>Bits 8:0 - a signed number that represents the offset for writing trigger bits to trigger memory.  Use this to adjust if ROI is off by a bit.  Bits 15:9 unused</t>
+  </si>
+  <si>
+    <t>Bits 7:0 timing reg (ASIC register), Bit 8: Signal for the sampling block to perform the sync  - set to one after all taps/biases are programmed, Bits 10:9 Choose which phase to use among 4 PHAB phases, Bit 11: toggle between two possible choices for WR_ADDR LSB phase</t>
+  </si>
+  <si>
+    <t>Firmware revision</t>
+  </si>
+  <si>
+    <t>Should match the repository revision number</t>
   </si>
 </sst>
 </file>
@@ -1927,9 +1933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H190" sqref="H190"/>
+    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F383" sqref="F383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6709,7 +6715,7 @@
         <v>85</v>
       </c>
       <c r="H189" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="190" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -11719,13 +11725,13 @@
         <v>5</v>
       </c>
       <c r="F381" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G381" s="5" t="s">
         <v>188</v>
       </c>
       <c r="H381" s="5" t="s">
-        <v>405</v>
+        <v>440</v>
       </c>
     </row>
     <row r="382" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -11746,13 +11752,13 @@
         <v>10</v>
       </c>
       <c r="F382" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G382" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H382" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -13906,9 +13912,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H628"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A610" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G613" sqref="G613"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26481,7 +26487,7 @@
       </c>
       <c r="H381" s="8" t="str">
         <f>'SCROD Write Registers'!H381</f>
-        <v>Bits 7:0 timing reg (ASIC register), Bit 8: Signal for the sampling block to perform the sync  - set to one after all taps/biases are programmed, Bits 10:9 Choose which phase to use among 4 PHAB phases</v>
+        <v>Bits 7:0 timing reg (ASIC register), Bit 8: Signal for the sampling block to perform the sync  - set to one after all taps/biases are programmed, Bits 10:9 Choose which phase to use among 4 PHAB phases, Bit 11: toggle between two possible choices for WR_ADDR LSB phase</v>
       </c>
     </row>
     <row r="382" spans="1:8" x14ac:dyDescent="0.25">
@@ -33480,17 +33486,41 @@
         <v>10</v>
       </c>
       <c r="F612" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="G612" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="G612" s="5" t="s">
+      <c r="H612" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="H612" s="5" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="613" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B613" s="3"/>
+    </row>
+    <row r="613" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A613" s="5">
+        <v>611</v>
+      </c>
+      <c r="B613" s="6" t="str">
+        <f t="shared" ref="B613" si="13">DEC2HEX(A613,4)</f>
+        <v>0263</v>
+      </c>
+      <c r="C613" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D613" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E613" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F613" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="G613" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H613" s="5" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="614" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B614" s="3"/>
@@ -34719,7 +34749,7 @@
         <v>267</v>
       </c>
       <c r="N41" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O41">
         <f t="shared" si="0"/>
@@ -34893,7 +34923,7 @@
         <v>253</v>
       </c>
       <c r="N47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="O47">
         <f t="shared" si="0"/>
@@ -34952,7 +34982,7 @@
         <v>247</v>
       </c>
       <c r="N49" s="54" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="O49">
         <f t="shared" si="0"/>
@@ -35011,7 +35041,7 @@
         <v>240</v>
       </c>
       <c r="N51" s="55" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="O51">
         <f t="shared" si="0"/>
@@ -35720,16 +35750,16 @@
         <v>171</v>
       </c>
       <c r="B3" s="46" t="s">
+        <v>411</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>412</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="D3" s="46" t="s">
         <v>413</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="E3" s="46" t="s">
         <v>414</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>415</v>
       </c>
       <c r="F3" s="47"/>
       <c r="H3" s="47"/>
@@ -35744,7 +35774,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="48" t="s">
         <v>173</v>
@@ -35769,7 +35799,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
@@ -35790,7 +35820,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
@@ -35811,13 +35841,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="46" t="s">
+        <v>418</v>
+      </c>
+      <c r="C7" s="46" t="s">
         <v>419</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="D7" s="46" t="s">
         <v>420</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>421</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>179</v>
@@ -35835,13 +35865,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="46" t="s">
+        <v>421</v>
+      </c>
+      <c r="C8" s="46" t="s">
         <v>422</v>
       </c>
-      <c r="C8" s="46" t="s">
-        <v>423</v>
-      </c>
       <c r="D8" s="46" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E8" s="46" t="s">
         <v>181</v>
@@ -35859,13 +35889,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="46" t="s">
+        <v>423</v>
+      </c>
+      <c r="C9" s="46" t="s">
         <v>424</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="D9" s="46" t="s">
         <v>425</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>426</v>
       </c>
       <c r="E9" s="46" t="s">
         <v>182</v>
@@ -35883,13 +35913,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="46" t="s">
+        <v>426</v>
+      </c>
+      <c r="C10" s="46" t="s">
         <v>427</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="D10" s="46" t="s">
         <v>428</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>429</v>
       </c>
       <c r="E10" s="46" t="s">
         <v>184</v>
@@ -35907,13 +35937,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="46" t="s">
+        <v>429</v>
+      </c>
+      <c r="C11" s="46" t="s">
         <v>430</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="D11" s="46" t="s">
         <v>431</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>432</v>
       </c>
       <c r="E11" s="46" t="s">
         <v>186</v>
@@ -35945,16 +35975,16 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="46" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D16" s="46" t="s">
+        <v>432</v>
+      </c>
+      <c r="E16" s="53" t="s">
         <v>433</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>434</v>
       </c>
       <c r="F16" s="53"/>
       <c r="G16" s="47"/>

</xml_diff>

<commit_message>
Added first stab at WBIAS/Trigger width monitoring and feedback.  Added extra MUX functionality to MON2 to allow looking at different bits of the write address on that pin, as an alternative to looking at MONTIMING2.  These MUX signals are controlled with register 380.  Register map updated.  Revision number updated.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="11280" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="11280" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD Write Registers" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2624" uniqueCount="466">
   <si>
     <t>Register Number</t>
   </si>
@@ -1338,9 +1338,6 @@
     <t>AD0</t>
   </si>
   <si>
-    <t>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 4: choose between MONTIMING and RCOSSX, bits 9:8 row select for MONTIMING2, bits 11:10 col select for MONTIMING2</t>
-  </si>
-  <si>
     <t>Bits 8:0 - a signed number that represents the offset for writing trigger bits to trigger memory.  Use this to adjust if ROI is off by a bit.  Bits 15:9 unused</t>
   </si>
   <si>
@@ -1351,6 +1348,78 @@
   </si>
   <si>
     <t>Should match the repository revision number</t>
+  </si>
+  <si>
+    <t>TRIG_WIDTH_COUNTER</t>
+  </si>
+  <si>
+    <t>WBIAS_FB</t>
+  </si>
+  <si>
+    <t>Feedback DAC value of WBIAS</t>
+  </si>
+  <si>
+    <t>see reg 628</t>
+  </si>
+  <si>
+    <t>see reg 612</t>
+  </si>
+  <si>
+    <t>Trigger width counter</t>
+  </si>
+  <si>
+    <t>Target count rate value for trigger-width counter feedback loop</t>
+  </si>
+  <si>
+    <t>TRIG_WIDTH_TARGET</t>
+  </si>
+  <si>
+    <t>17 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>18 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>19 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>20 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>21 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>22 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>23 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>24 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>25 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>26 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>27 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>28 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>29 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>30 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>31 bit unsigned counter</t>
+  </si>
+  <si>
+    <t>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 4: choose between MONTIMING and RCOSSX, bits 9:8 row select for MONTIMING2, bits 11:10 col select for MONTIMING2, bit 12: when '0' put MONTIMING for second ASIC on MON2, when '1' put WR_ADDR on MON2; bits15:13 choose which WR_ADDR bit to put on MON2</t>
   </si>
 </sst>
 </file>
@@ -1933,9 +2002,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F383" sqref="F383"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H383" sqref="H383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6715,7 +6784,7 @@
         <v>85</v>
       </c>
       <c r="H189" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="190" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -11731,7 +11800,7 @@
         <v>188</v>
       </c>
       <c r="H381" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="382" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -11758,7 +11827,7 @@
         <v>408</v>
       </c>
       <c r="H382" s="5" t="s">
-        <v>438</v>
+        <v>465</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -12688,199 +12757,439 @@
         <v>222</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A419">
+    <row r="419" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A419" s="5">
         <v>417</v>
       </c>
-      <c r="B419" s="4" t="str">
+      <c r="B419" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A1</v>
       </c>
-      <c r="F419" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A420">
+      <c r="C419" s="5">
+        <v>0</v>
+      </c>
+      <c r="D419" s="5">
+        <v>0</v>
+      </c>
+      <c r="E419" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F419" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G419" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H419" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="420" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A420" s="5">
         <v>418</v>
       </c>
-      <c r="B420" s="4" t="str">
+      <c r="B420" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A2</v>
       </c>
-      <c r="F420" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A421">
+      <c r="C420" s="5">
+        <v>0</v>
+      </c>
+      <c r="D420" s="5">
+        <v>1</v>
+      </c>
+      <c r="E420" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F420" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G420" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H420" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="421" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A421" s="5">
         <v>419</v>
       </c>
-      <c r="B421" s="4" t="str">
+      <c r="B421" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A3</v>
       </c>
-      <c r="F421" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A422">
+      <c r="C421" s="5">
+        <v>0</v>
+      </c>
+      <c r="D421" s="5">
+        <v>2</v>
+      </c>
+      <c r="E421" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F421" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G421" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H421" s="5" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="422" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A422" s="5">
         <v>420</v>
       </c>
-      <c r="B422" s="4" t="str">
+      <c r="B422" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A4</v>
       </c>
-      <c r="F422" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A423">
+      <c r="C422" s="5">
+        <v>0</v>
+      </c>
+      <c r="D422" s="5">
+        <v>3</v>
+      </c>
+      <c r="E422" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F422" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G422" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H422" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="423" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A423" s="5">
         <v>421</v>
       </c>
-      <c r="B423" s="4" t="str">
+      <c r="B423" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A5</v>
       </c>
-      <c r="F423" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A424">
+      <c r="C423" s="5">
+        <v>1</v>
+      </c>
+      <c r="D423" s="5">
+        <v>0</v>
+      </c>
+      <c r="E423" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F423" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G423" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H423" s="5" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="424" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A424" s="5">
         <v>422</v>
       </c>
-      <c r="B424" s="4" t="str">
+      <c r="B424" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A6</v>
       </c>
-      <c r="F424" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A425">
+      <c r="C424" s="5">
+        <v>1</v>
+      </c>
+      <c r="D424" s="5">
+        <v>1</v>
+      </c>
+      <c r="E424" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F424" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G424" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H424" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="425" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A425" s="5">
         <v>423</v>
       </c>
-      <c r="B425" s="4" t="str">
+      <c r="B425" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A7</v>
       </c>
-      <c r="F425" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A426">
+      <c r="C425" s="5">
+        <v>1</v>
+      </c>
+      <c r="D425" s="5">
+        <v>2</v>
+      </c>
+      <c r="E425" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F425" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G425" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H425" s="5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="426" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A426" s="5">
         <v>424</v>
       </c>
-      <c r="B426" s="4" t="str">
+      <c r="B426" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A8</v>
       </c>
-      <c r="F426" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A427">
+      <c r="C426" s="5">
+        <v>1</v>
+      </c>
+      <c r="D426" s="5">
+        <v>3</v>
+      </c>
+      <c r="E426" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F426" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G426" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H426" s="5" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="427" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A427" s="5">
         <v>425</v>
       </c>
-      <c r="B427" s="4" t="str">
+      <c r="B427" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01A9</v>
       </c>
-      <c r="F427" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A428">
+      <c r="C427" s="5">
+        <v>2</v>
+      </c>
+      <c r="D427" s="5">
+        <v>0</v>
+      </c>
+      <c r="E427" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F427" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G427" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H427" s="5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="428" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A428" s="5">
         <v>426</v>
       </c>
-      <c r="B428" s="4" t="str">
+      <c r="B428" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01AA</v>
       </c>
-      <c r="F428" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A429">
+      <c r="C428" s="5">
+        <v>2</v>
+      </c>
+      <c r="D428" s="5">
+        <v>1</v>
+      </c>
+      <c r="E428" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F428" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G428" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H428" s="5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="429" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A429" s="5">
         <v>427</v>
       </c>
-      <c r="B429" s="4" t="str">
+      <c r="B429" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01AB</v>
       </c>
-      <c r="F429" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A430">
+      <c r="C429" s="5">
+        <v>2</v>
+      </c>
+      <c r="D429" s="5">
+        <v>2</v>
+      </c>
+      <c r="E429" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F429" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G429" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H429" s="5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="430" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A430" s="5">
         <v>428</v>
       </c>
-      <c r="B430" s="4" t="str">
+      <c r="B430" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01AC</v>
       </c>
-      <c r="F430" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A431">
+      <c r="C430" s="5">
+        <v>2</v>
+      </c>
+      <c r="D430" s="5">
+        <v>3</v>
+      </c>
+      <c r="E430" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F430" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G430" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H430" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="431" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A431" s="5">
         <v>429</v>
       </c>
-      <c r="B431" s="4" t="str">
+      <c r="B431" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01AD</v>
       </c>
-      <c r="F431" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A432">
+      <c r="C431" s="5">
+        <v>3</v>
+      </c>
+      <c r="D431" s="5">
+        <v>0</v>
+      </c>
+      <c r="E431" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F431" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G431" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H431" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="432" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A432" s="5">
         <v>430</v>
       </c>
-      <c r="B432" s="4" t="str">
+      <c r="B432" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01AE</v>
       </c>
-      <c r="F432" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A433">
+      <c r="C432" s="5">
+        <v>3</v>
+      </c>
+      <c r="D432" s="5">
+        <v>1</v>
+      </c>
+      <c r="E432" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F432" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G432" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H432" s="5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="433" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A433" s="5">
         <v>431</v>
       </c>
-      <c r="B433" s="4" t="str">
+      <c r="B433" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01AF</v>
       </c>
-      <c r="F433" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A434">
+      <c r="C433" s="5">
+        <v>3</v>
+      </c>
+      <c r="D433" s="5">
+        <v>2</v>
+      </c>
+      <c r="E433" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F433" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G433" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H433" s="5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="434" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A434" s="5">
         <v>432</v>
       </c>
-      <c r="B434" s="4" t="str">
+      <c r="B434" s="7" t="str">
         <f t="shared" si="8"/>
         <v>01B0</v>
       </c>
-      <c r="F434" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C434" s="5">
+        <v>3</v>
+      </c>
+      <c r="D434" s="5">
+        <v>3</v>
+      </c>
+      <c r="E434" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F434" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G434" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="H434" s="5" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>433</v>
       </c>
@@ -12892,7 +13201,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>434</v>
       </c>
@@ -12904,7 +13213,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>435</v>
       </c>
@@ -12916,7 +13225,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>436</v>
       </c>
@@ -12928,7 +13237,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>437</v>
       </c>
@@ -12940,7 +13249,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>438</v>
       </c>
@@ -12952,7 +13261,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>439</v>
       </c>
@@ -12964,7 +13273,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>440</v>
       </c>
@@ -12976,7 +13285,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>441</v>
       </c>
@@ -12988,7 +13297,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>442</v>
       </c>
@@ -13000,7 +13309,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>443</v>
       </c>
@@ -13012,7 +13321,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>444</v>
       </c>
@@ -13024,7 +13333,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>445</v>
       </c>
@@ -13036,7 +13345,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>446</v>
       </c>
@@ -13910,11 +14219,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H628"/>
+  <dimension ref="A1:H649"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A610" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G613" sqref="G613"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A506" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F527" sqref="F527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26520,7 +26829,7 @@
       </c>
       <c r="H382" s="8" t="str">
         <f>'SCROD Write Registers'!H382</f>
-        <v>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 4: choose between MONTIMING and RCOSSX, bits 9:8 row select for MONTIMING2, bits 11:10 col select for MONTIMING2</v>
+        <v>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 4: choose between MONTIMING and RCOSSX, bits 9:8 row select for MONTIMING2, bits 11:10 col select for MONTIMING2, bit 12: when '0' put MONTIMING for second ASIC on MON2, when '1' put WR_ADDR on MON2; bits15:13 choose which WR_ADDR bit to put on MON2</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -27727,21 +28036,21 @@
         <f>'SCROD Write Registers'!D419</f>
         <v>0</v>
       </c>
-      <c r="E419">
+      <c r="E419" t="str">
         <f>'SCROD Write Registers'!E419</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F419" t="str">
         <f>'SCROD Write Registers'!F419</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G419" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G419" s="8" t="str">
         <f>'SCROD Write Registers'!G419</f>
-        <v>0</v>
-      </c>
-      <c r="H419" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H419" s="8" t="str">
         <f>'SCROD Write Registers'!H419</f>
-        <v>0</v>
+        <v>16 bit unsigned counter</v>
       </c>
     </row>
     <row r="420" spans="1:8" x14ac:dyDescent="0.25">
@@ -27758,23 +28067,23 @@
       </c>
       <c r="D420">
         <f>'SCROD Write Registers'!D420</f>
-        <v>0</v>
-      </c>
-      <c r="E420">
+        <v>1</v>
+      </c>
+      <c r="E420" t="str">
         <f>'SCROD Write Registers'!E420</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F420" t="str">
         <f>'SCROD Write Registers'!F420</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G420" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G420" s="8" t="str">
         <f>'SCROD Write Registers'!G420</f>
-        <v>0</v>
-      </c>
-      <c r="H420" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H420" s="8" t="str">
         <f>'SCROD Write Registers'!H420</f>
-        <v>0</v>
+        <v>17 bit unsigned counter</v>
       </c>
     </row>
     <row r="421" spans="1:8" x14ac:dyDescent="0.25">
@@ -27791,23 +28100,23 @@
       </c>
       <c r="D421">
         <f>'SCROD Write Registers'!D421</f>
-        <v>0</v>
-      </c>
-      <c r="E421">
+        <v>2</v>
+      </c>
+      <c r="E421" t="str">
         <f>'SCROD Write Registers'!E421</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F421" t="str">
         <f>'SCROD Write Registers'!F421</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G421" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G421" s="8" t="str">
         <f>'SCROD Write Registers'!G421</f>
-        <v>0</v>
-      </c>
-      <c r="H421" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H421" s="8" t="str">
         <f>'SCROD Write Registers'!H421</f>
-        <v>0</v>
+        <v>18 bit unsigned counter</v>
       </c>
     </row>
     <row r="422" spans="1:8" x14ac:dyDescent="0.25">
@@ -27824,23 +28133,23 @@
       </c>
       <c r="D422">
         <f>'SCROD Write Registers'!D422</f>
-        <v>0</v>
-      </c>
-      <c r="E422">
+        <v>3</v>
+      </c>
+      <c r="E422" t="str">
         <f>'SCROD Write Registers'!E422</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F422" t="str">
         <f>'SCROD Write Registers'!F422</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G422" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G422" s="8" t="str">
         <f>'SCROD Write Registers'!G422</f>
-        <v>0</v>
-      </c>
-      <c r="H422" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H422" s="8" t="str">
         <f>'SCROD Write Registers'!H422</f>
-        <v>0</v>
+        <v>19 bit unsigned counter</v>
       </c>
     </row>
     <row r="423" spans="1:8" x14ac:dyDescent="0.25">
@@ -27853,27 +28162,27 @@
       </c>
       <c r="C423">
         <f>'SCROD Write Registers'!C423</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D423">
         <f>'SCROD Write Registers'!D423</f>
         <v>0</v>
       </c>
-      <c r="E423">
+      <c r="E423" t="str">
         <f>'SCROD Write Registers'!E423</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F423" t="str">
         <f>'SCROD Write Registers'!F423</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G423" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G423" s="8" t="str">
         <f>'SCROD Write Registers'!G423</f>
-        <v>0</v>
-      </c>
-      <c r="H423" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H423" s="8" t="str">
         <f>'SCROD Write Registers'!H423</f>
-        <v>0</v>
+        <v>20 bit unsigned counter</v>
       </c>
     </row>
     <row r="424" spans="1:8" x14ac:dyDescent="0.25">
@@ -27886,27 +28195,27 @@
       </c>
       <c r="C424">
         <f>'SCROD Write Registers'!C424</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D424">
         <f>'SCROD Write Registers'!D424</f>
-        <v>0</v>
-      </c>
-      <c r="E424">
+        <v>1</v>
+      </c>
+      <c r="E424" t="str">
         <f>'SCROD Write Registers'!E424</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F424" t="str">
         <f>'SCROD Write Registers'!F424</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G424" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G424" s="8" t="str">
         <f>'SCROD Write Registers'!G424</f>
-        <v>0</v>
-      </c>
-      <c r="H424" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H424" s="8" t="str">
         <f>'SCROD Write Registers'!H424</f>
-        <v>0</v>
+        <v>21 bit unsigned counter</v>
       </c>
     </row>
     <row r="425" spans="1:8" x14ac:dyDescent="0.25">
@@ -27919,27 +28228,27 @@
       </c>
       <c r="C425">
         <f>'SCROD Write Registers'!C425</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D425">
         <f>'SCROD Write Registers'!D425</f>
-        <v>0</v>
-      </c>
-      <c r="E425">
+        <v>2</v>
+      </c>
+      <c r="E425" t="str">
         <f>'SCROD Write Registers'!E425</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F425" t="str">
         <f>'SCROD Write Registers'!F425</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G425" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G425" s="8" t="str">
         <f>'SCROD Write Registers'!G425</f>
-        <v>0</v>
-      </c>
-      <c r="H425" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H425" s="8" t="str">
         <f>'SCROD Write Registers'!H425</f>
-        <v>0</v>
+        <v>22 bit unsigned counter</v>
       </c>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.25">
@@ -27952,27 +28261,27 @@
       </c>
       <c r="C426">
         <f>'SCROD Write Registers'!C426</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D426">
         <f>'SCROD Write Registers'!D426</f>
-        <v>0</v>
-      </c>
-      <c r="E426">
+        <v>3</v>
+      </c>
+      <c r="E426" t="str">
         <f>'SCROD Write Registers'!E426</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F426" t="str">
         <f>'SCROD Write Registers'!F426</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G426" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G426" s="8" t="str">
         <f>'SCROD Write Registers'!G426</f>
-        <v>0</v>
-      </c>
-      <c r="H426" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H426" s="8" t="str">
         <f>'SCROD Write Registers'!H426</f>
-        <v>0</v>
+        <v>23 bit unsigned counter</v>
       </c>
     </row>
     <row r="427" spans="1:8" x14ac:dyDescent="0.25">
@@ -27985,27 +28294,27 @@
       </c>
       <c r="C427">
         <f>'SCROD Write Registers'!C427</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D427">
         <f>'SCROD Write Registers'!D427</f>
         <v>0</v>
       </c>
-      <c r="E427">
+      <c r="E427" t="str">
         <f>'SCROD Write Registers'!E427</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F427" t="str">
         <f>'SCROD Write Registers'!F427</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G427" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G427" s="8" t="str">
         <f>'SCROD Write Registers'!G427</f>
-        <v>0</v>
-      </c>
-      <c r="H427" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H427" s="8" t="str">
         <f>'SCROD Write Registers'!H427</f>
-        <v>0</v>
+        <v>24 bit unsigned counter</v>
       </c>
     </row>
     <row r="428" spans="1:8" x14ac:dyDescent="0.25">
@@ -28018,27 +28327,27 @@
       </c>
       <c r="C428">
         <f>'SCROD Write Registers'!C428</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D428">
         <f>'SCROD Write Registers'!D428</f>
-        <v>0</v>
-      </c>
-      <c r="E428">
+        <v>1</v>
+      </c>
+      <c r="E428" t="str">
         <f>'SCROD Write Registers'!E428</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F428" t="str">
         <f>'SCROD Write Registers'!F428</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G428" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G428" s="8" t="str">
         <f>'SCROD Write Registers'!G428</f>
-        <v>0</v>
-      </c>
-      <c r="H428" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H428" s="8" t="str">
         <f>'SCROD Write Registers'!H428</f>
-        <v>0</v>
+        <v>25 bit unsigned counter</v>
       </c>
     </row>
     <row r="429" spans="1:8" x14ac:dyDescent="0.25">
@@ -28051,27 +28360,27 @@
       </c>
       <c r="C429">
         <f>'SCROD Write Registers'!C429</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D429">
         <f>'SCROD Write Registers'!D429</f>
-        <v>0</v>
-      </c>
-      <c r="E429">
+        <v>2</v>
+      </c>
+      <c r="E429" t="str">
         <f>'SCROD Write Registers'!E429</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F429" t="str">
         <f>'SCROD Write Registers'!F429</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G429" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G429" s="8" t="str">
         <f>'SCROD Write Registers'!G429</f>
-        <v>0</v>
-      </c>
-      <c r="H429" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H429" s="8" t="str">
         <f>'SCROD Write Registers'!H429</f>
-        <v>0</v>
+        <v>26 bit unsigned counter</v>
       </c>
     </row>
     <row r="430" spans="1:8" x14ac:dyDescent="0.25">
@@ -28084,27 +28393,27 @@
       </c>
       <c r="C430">
         <f>'SCROD Write Registers'!C430</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D430">
         <f>'SCROD Write Registers'!D430</f>
-        <v>0</v>
-      </c>
-      <c r="E430">
+        <v>3</v>
+      </c>
+      <c r="E430" t="str">
         <f>'SCROD Write Registers'!E430</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F430" t="str">
         <f>'SCROD Write Registers'!F430</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G430" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G430" s="8" t="str">
         <f>'SCROD Write Registers'!G430</f>
-        <v>0</v>
-      </c>
-      <c r="H430" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H430" s="8" t="str">
         <f>'SCROD Write Registers'!H430</f>
-        <v>0</v>
+        <v>27 bit unsigned counter</v>
       </c>
     </row>
     <row r="431" spans="1:8" x14ac:dyDescent="0.25">
@@ -28117,27 +28426,27 @@
       </c>
       <c r="C431">
         <f>'SCROD Write Registers'!C431</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D431">
         <f>'SCROD Write Registers'!D431</f>
         <v>0</v>
       </c>
-      <c r="E431">
+      <c r="E431" t="str">
         <f>'SCROD Write Registers'!E431</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F431" t="str">
         <f>'SCROD Write Registers'!F431</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G431" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G431" s="8" t="str">
         <f>'SCROD Write Registers'!G431</f>
-        <v>0</v>
-      </c>
-      <c r="H431" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H431" s="8" t="str">
         <f>'SCROD Write Registers'!H431</f>
-        <v>0</v>
+        <v>28 bit unsigned counter</v>
       </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.25">
@@ -28150,27 +28459,27 @@
       </c>
       <c r="C432">
         <f>'SCROD Write Registers'!C432</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D432">
         <f>'SCROD Write Registers'!D432</f>
-        <v>0</v>
-      </c>
-      <c r="E432">
+        <v>1</v>
+      </c>
+      <c r="E432" t="str">
         <f>'SCROD Write Registers'!E432</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F432" t="str">
         <f>'SCROD Write Registers'!F432</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G432" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G432" s="8" t="str">
         <f>'SCROD Write Registers'!G432</f>
-        <v>0</v>
-      </c>
-      <c r="H432" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H432" s="8" t="str">
         <f>'SCROD Write Registers'!H432</f>
-        <v>0</v>
+        <v>29 bit unsigned counter</v>
       </c>
     </row>
     <row r="433" spans="1:8" x14ac:dyDescent="0.25">
@@ -28183,27 +28492,27 @@
       </c>
       <c r="C433">
         <f>'SCROD Write Registers'!C433</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D433">
         <f>'SCROD Write Registers'!D433</f>
-        <v>0</v>
-      </c>
-      <c r="E433">
+        <v>2</v>
+      </c>
+      <c r="E433" t="str">
         <f>'SCROD Write Registers'!E433</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F433" t="str">
         <f>'SCROD Write Registers'!F433</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G433" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G433" s="8" t="str">
         <f>'SCROD Write Registers'!G433</f>
-        <v>0</v>
-      </c>
-      <c r="H433" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H433" s="8" t="str">
         <f>'SCROD Write Registers'!H433</f>
-        <v>0</v>
+        <v>30 bit unsigned counter</v>
       </c>
     </row>
     <row r="434" spans="1:8" x14ac:dyDescent="0.25">
@@ -28216,27 +28525,27 @@
       </c>
       <c r="C434">
         <f>'SCROD Write Registers'!C434</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D434">
         <f>'SCROD Write Registers'!D434</f>
-        <v>0</v>
-      </c>
-      <c r="E434">
+        <v>3</v>
+      </c>
+      <c r="E434" t="str">
         <f>'SCROD Write Registers'!E434</f>
-        <v>0</v>
+        <v>G</v>
       </c>
       <c r="F434" t="str">
         <f>'SCROD Write Registers'!F434</f>
-        <v>Reserved (but not yet used)</v>
-      </c>
-      <c r="G434" s="8">
+        <v>TRIG_WIDTH_TARGET</v>
+      </c>
+      <c r="G434" s="8" t="str">
         <f>'SCROD Write Registers'!G434</f>
-        <v>0</v>
-      </c>
-      <c r="H434" s="8">
+        <v>Target count rate value for trigger-width counter feedback loop</v>
+      </c>
+      <c r="H434" s="8" t="str">
         <f>'SCROD Write Registers'!H434</f>
-        <v>0</v>
+        <v>31 bit unsigned counter</v>
       </c>
     </row>
     <row r="435" spans="1:8" x14ac:dyDescent="0.25">
@@ -33500,7 +33809,7 @@
         <v>611</v>
       </c>
       <c r="B613" s="6" t="str">
-        <f t="shared" ref="B613" si="13">DEC2HEX(A613,4)</f>
+        <f t="shared" ref="B613:B649" si="13">DEC2HEX(A613,4)</f>
         <v>0263</v>
       </c>
       <c r="C613" s="5" t="s">
@@ -33513,59 +33822,851 @@
         <v>10</v>
       </c>
       <c r="F613" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="G613" s="5" t="s">
         <v>441</v>
-      </c>
-      <c r="G613" s="5" t="s">
-        <v>442</v>
       </c>
       <c r="H613" s="5" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="614" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B614" s="3"/>
-    </row>
-    <row r="615" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B615" s="3"/>
-    </row>
-    <row r="616" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B616" s="3"/>
-    </row>
-    <row r="617" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B617" s="3"/>
-    </row>
-    <row r="618" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B618" s="3"/>
-    </row>
-    <row r="619" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B619" s="3"/>
-    </row>
-    <row r="620" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B620" s="3"/>
-    </row>
-    <row r="621" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B621" s="3"/>
-    </row>
-    <row r="622" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B622" s="3"/>
-    </row>
-    <row r="623" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B623" s="3"/>
-    </row>
-    <row r="624" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B624" s="3"/>
-    </row>
-    <row r="625" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B625" s="3"/>
-    </row>
-    <row r="626" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B626" s="3"/>
-    </row>
-    <row r="627" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B627" s="3"/>
-    </row>
-    <row r="628" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B628" s="3"/>
+    <row r="614" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A614" s="5">
+        <v>612</v>
+      </c>
+      <c r="B614" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0264</v>
+      </c>
+      <c r="C614" s="5">
+        <v>0</v>
+      </c>
+      <c r="D614" s="5">
+        <v>0</v>
+      </c>
+      <c r="E614" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F614" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="G614" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="H614" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="615" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A615" s="5">
+        <v>613</v>
+      </c>
+      <c r="B615" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0265</v>
+      </c>
+      <c r="C615" s="5">
+        <v>0</v>
+      </c>
+      <c r="D615" s="5">
+        <v>1</v>
+      </c>
+      <c r="E615" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F615" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="G615" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="H615" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="616" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A616" s="5">
+        <v>614</v>
+      </c>
+      <c r="B616" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0266</v>
+      </c>
+      <c r="C616" s="5">
+        <v>0</v>
+      </c>
+      <c r="D616" s="5">
+        <v>2</v>
+      </c>
+      <c r="E616" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F616" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="G616" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="H616" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="617" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A617" s="5">
+        <v>615</v>
+      </c>
+      <c r="B617" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0267</v>
+      </c>
+      <c r="C617" s="5">
+        <v>0</v>
+      </c>
+      <c r="D617" s="5">
+        <v>3</v>
+      </c>
+      <c r="E617" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F617" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H617" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="618" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A618" s="5">
+        <v>616</v>
+      </c>
+      <c r="B618" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0268</v>
+      </c>
+      <c r="C618" s="5">
+        <v>1</v>
+      </c>
+      <c r="D618" s="5">
+        <v>0</v>
+      </c>
+      <c r="E618" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F618" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H618" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="619" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A619" s="5">
+        <v>617</v>
+      </c>
+      <c r="B619" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0269</v>
+      </c>
+      <c r="C619" s="5">
+        <v>1</v>
+      </c>
+      <c r="D619" s="5">
+        <v>1</v>
+      </c>
+      <c r="E619" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F619" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H619" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="620" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A620" s="5">
+        <v>618</v>
+      </c>
+      <c r="B620" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>026A</v>
+      </c>
+      <c r="C620" s="5">
+        <v>1</v>
+      </c>
+      <c r="D620" s="5">
+        <v>2</v>
+      </c>
+      <c r="E620" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F620" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H620" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="621" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A621" s="5">
+        <v>619</v>
+      </c>
+      <c r="B621" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>026B</v>
+      </c>
+      <c r="C621" s="5">
+        <v>1</v>
+      </c>
+      <c r="D621" s="5">
+        <v>3</v>
+      </c>
+      <c r="E621" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F621" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H621" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="622" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A622" s="5">
+        <v>620</v>
+      </c>
+      <c r="B622" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>026C</v>
+      </c>
+      <c r="C622" s="5">
+        <v>2</v>
+      </c>
+      <c r="D622" s="5">
+        <v>0</v>
+      </c>
+      <c r="E622" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F622" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H622" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="623" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A623" s="5">
+        <v>621</v>
+      </c>
+      <c r="B623" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>026D</v>
+      </c>
+      <c r="C623" s="5">
+        <v>2</v>
+      </c>
+      <c r="D623" s="5">
+        <v>1</v>
+      </c>
+      <c r="E623" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F623" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H623" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="624" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A624" s="5">
+        <v>622</v>
+      </c>
+      <c r="B624" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>026E</v>
+      </c>
+      <c r="C624" s="5">
+        <v>2</v>
+      </c>
+      <c r="D624" s="5">
+        <v>2</v>
+      </c>
+      <c r="E624" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F624" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H624" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="625" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A625" s="5">
+        <v>623</v>
+      </c>
+      <c r="B625" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>026F</v>
+      </c>
+      <c r="C625" s="5">
+        <v>2</v>
+      </c>
+      <c r="D625" s="5">
+        <v>3</v>
+      </c>
+      <c r="E625" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F625" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H625" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="626" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A626" s="5">
+        <v>624</v>
+      </c>
+      <c r="B626" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0270</v>
+      </c>
+      <c r="C626" s="5">
+        <v>3</v>
+      </c>
+      <c r="D626" s="5">
+        <v>0</v>
+      </c>
+      <c r="E626" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F626" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H626" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="627" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A627" s="5">
+        <v>625</v>
+      </c>
+      <c r="B627" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0271</v>
+      </c>
+      <c r="C627" s="5">
+        <v>3</v>
+      </c>
+      <c r="D627" s="5">
+        <v>1</v>
+      </c>
+      <c r="E627" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F627" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H627" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="628" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A628" s="5">
+        <v>626</v>
+      </c>
+      <c r="B628" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0272</v>
+      </c>
+      <c r="C628" s="5">
+        <v>3</v>
+      </c>
+      <c r="D628" s="5">
+        <v>2</v>
+      </c>
+      <c r="E628" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F628" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H628" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="629" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A629" s="5">
+        <v>627</v>
+      </c>
+      <c r="B629" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0273</v>
+      </c>
+      <c r="C629" s="5">
+        <v>3</v>
+      </c>
+      <c r="D629" s="5">
+        <v>3</v>
+      </c>
+      <c r="E629" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F629" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H629" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="630" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A630" s="5">
+        <v>628</v>
+      </c>
+      <c r="B630" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0274</v>
+      </c>
+      <c r="C630" s="5">
+        <v>0</v>
+      </c>
+      <c r="D630" s="5">
+        <v>0</v>
+      </c>
+      <c r="E630" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F630" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G630" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="H630" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="631" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A631" s="5">
+        <v>629</v>
+      </c>
+      <c r="B631" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0275</v>
+      </c>
+      <c r="C631" s="5">
+        <v>0</v>
+      </c>
+      <c r="D631" s="5">
+        <v>1</v>
+      </c>
+      <c r="E631" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F631" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G631" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H631" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="632" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A632" s="5">
+        <v>630</v>
+      </c>
+      <c r="B632" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0276</v>
+      </c>
+      <c r="C632" s="5">
+        <v>0</v>
+      </c>
+      <c r="D632" s="5">
+        <v>0</v>
+      </c>
+      <c r="E632" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F632" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G632" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H632" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="633" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A633" s="5">
+        <v>631</v>
+      </c>
+      <c r="B633" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0277</v>
+      </c>
+      <c r="C633" s="5">
+        <v>0</v>
+      </c>
+      <c r="D633" s="5">
+        <v>1</v>
+      </c>
+      <c r="E633" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F633" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G633" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H633" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="634" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A634" s="5">
+        <v>632</v>
+      </c>
+      <c r="B634" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0278</v>
+      </c>
+      <c r="C634" s="5">
+        <v>0</v>
+      </c>
+      <c r="D634" s="5">
+        <v>2</v>
+      </c>
+      <c r="E634" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F634" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G634" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H634" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="635" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A635" s="5">
+        <v>633</v>
+      </c>
+      <c r="B635" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0279</v>
+      </c>
+      <c r="C635" s="5">
+        <v>0</v>
+      </c>
+      <c r="D635" s="5">
+        <v>3</v>
+      </c>
+      <c r="E635" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F635" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G635" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H635" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="636" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A636" s="5">
+        <v>634</v>
+      </c>
+      <c r="B636" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>027A</v>
+      </c>
+      <c r="C636" s="5">
+        <v>1</v>
+      </c>
+      <c r="D636" s="5">
+        <v>0</v>
+      </c>
+      <c r="E636" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F636" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G636" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H636" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="637" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A637" s="5">
+        <v>635</v>
+      </c>
+      <c r="B637" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>027B</v>
+      </c>
+      <c r="C637" s="5">
+        <v>1</v>
+      </c>
+      <c r="D637" s="5">
+        <v>1</v>
+      </c>
+      <c r="E637" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F637" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G637" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H637" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="638" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A638" s="5">
+        <v>636</v>
+      </c>
+      <c r="B638" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>027C</v>
+      </c>
+      <c r="C638" s="5">
+        <v>1</v>
+      </c>
+      <c r="D638" s="5">
+        <v>2</v>
+      </c>
+      <c r="E638" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F638" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G638" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H638" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="639" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A639" s="5">
+        <v>637</v>
+      </c>
+      <c r="B639" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>027D</v>
+      </c>
+      <c r="C639" s="5">
+        <v>1</v>
+      </c>
+      <c r="D639" s="5">
+        <v>3</v>
+      </c>
+      <c r="E639" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F639" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G639" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H639" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="640" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A640" s="5">
+        <v>638</v>
+      </c>
+      <c r="B640" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>027E</v>
+      </c>
+      <c r="C640" s="5">
+        <v>2</v>
+      </c>
+      <c r="D640" s="5">
+        <v>0</v>
+      </c>
+      <c r="E640" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F640" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G640" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H640" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="641" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A641" s="5">
+        <v>639</v>
+      </c>
+      <c r="B641" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>027F</v>
+      </c>
+      <c r="C641" s="5">
+        <v>2</v>
+      </c>
+      <c r="D641" s="5">
+        <v>1</v>
+      </c>
+      <c r="E641" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F641" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G641" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H641" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="642" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A642" s="5">
+        <v>640</v>
+      </c>
+      <c r="B642" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0280</v>
+      </c>
+      <c r="C642" s="5">
+        <v>2</v>
+      </c>
+      <c r="D642" s="5">
+        <v>2</v>
+      </c>
+      <c r="E642" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F642" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G642" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H642" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="643" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A643" s="5">
+        <v>641</v>
+      </c>
+      <c r="B643" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0281</v>
+      </c>
+      <c r="C643" s="5">
+        <v>2</v>
+      </c>
+      <c r="D643" s="5">
+        <v>3</v>
+      </c>
+      <c r="E643" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F643" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G643" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H643" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="644" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A644" s="5">
+        <v>642</v>
+      </c>
+      <c r="B644" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0282</v>
+      </c>
+      <c r="C644" s="5">
+        <v>3</v>
+      </c>
+      <c r="D644" s="5">
+        <v>0</v>
+      </c>
+      <c r="E644" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F644" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G644" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H644" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="645" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A645" s="5">
+        <v>643</v>
+      </c>
+      <c r="B645" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0283</v>
+      </c>
+      <c r="C645" s="5">
+        <v>3</v>
+      </c>
+      <c r="D645" s="5">
+        <v>1</v>
+      </c>
+      <c r="E645" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F645" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G645" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H645" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="646" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B646" s="16"/>
+    </row>
+    <row r="647" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B647" s="16"/>
+    </row>
+    <row r="648" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B648" s="16"/>
+    </row>
+    <row r="649" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B649" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33597,7 +34698,7 @@
       </c>
       <c r="E1" s="26">
         <f ca="1">+TODAY()</f>
-        <v>41362</v>
+        <v>41364</v>
       </c>
       <c r="P1">
         <v>2500</v>

</xml_diff>

<commit_message>
Added a register to monitor the number of seconds the FTSW interface has been stable.  Updated the register map to reflect the addition.  Updated firmware revision number.
</commit_message>
<xml_diff>
--- a/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
+++ b/SCROD-boardstack/iTOP/IRS3B_CRT/contrib/register_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="11280" windowHeight="7965"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="11280" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD Write Registers" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2624" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2630" uniqueCount="453">
   <si>
     <t>Register Number</t>
   </si>
@@ -1375,6 +1375,12 @@
   </si>
   <si>
     <t>Bits 1:0 row select for MONTIMING/RCOSSX, bits 3:2 col select for MONTIMING/RCOSSX, bit 4: choose between MONTIMING and RCOSSX, bit 7  internal_MON2_OR_CAL_SELECT               &lt;= internal_OUTPUT_REGISTERS(380)(7);            -- bit      7 choose between MON_HEADER2 signal ('0') or CAL_PULSE ('1'); bits 9:8 row select for MONTIMING2, bits 11:10 col select for MONTIMING2, bit 12: when '0' put MONTIMING for second ASIC on MON2, when '1' put WR_ADDR on MON2; bits15:13 choose which WR_ADDR bit to put on MON2</t>
+  </si>
+  <si>
+    <t>Seconds FTSW locked</t>
+  </si>
+  <si>
+    <t>Number of seconds the FTSW stable signal has been high</t>
   </si>
 </sst>
 </file>
@@ -1600,41 +1606,8 @@
     <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -1645,13 +1618,46 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -1957,8 +1963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A421" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H383" sqref="H383"/>
     </sheetView>
   </sheetViews>
@@ -14176,9 +14182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H649"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A506" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A517" sqref="A517"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A617" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F631" sqref="F631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33764,7 +33770,7 @@
         <v>611</v>
       </c>
       <c r="B613" s="6" t="str">
-        <f t="shared" ref="B613:B649" si="13">DEC2HEX(A613,4)</f>
+        <f t="shared" ref="B613:B646" si="13">DEC2HEX(A613,4)</f>
         <v>0263</v>
       </c>
       <c r="C613" s="5" t="s">
@@ -34611,8 +34617,32 @@
         <v>28</v>
       </c>
     </row>
-    <row r="646" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B646" s="16"/>
+    <row r="646" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A646" s="5">
+        <v>644</v>
+      </c>
+      <c r="B646" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>0284</v>
+      </c>
+      <c r="C646" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D646" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E646" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F646" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="G646" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="H646" s="5" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="647" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B647" s="16"/>
@@ -34653,7 +34683,7 @@
       </c>
       <c r="E1" s="26">
         <f ca="1">+TODAY()</f>
-        <v>41367</v>
+        <v>41371</v>
       </c>
       <c r="P1">
         <v>2500</v>
@@ -34731,7 +34761,7 @@
       <c r="D6" s="24">
         <v>12</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="45" t="s">
         <v>343</v>
       </c>
       <c r="F6" s="24"/>
@@ -34767,7 +34797,7 @@
       <c r="D7" s="24">
         <v>12</v>
       </c>
-      <c r="E7" s="37"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
@@ -34801,7 +34831,7 @@
       <c r="D8" s="24">
         <v>12</v>
       </c>
-      <c r="E8" s="37"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
@@ -34835,7 +34865,7 @@
       <c r="D9" s="24">
         <v>12</v>
       </c>
-      <c r="E9" s="37"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
@@ -34869,7 +34899,7 @@
       <c r="D10" s="24">
         <v>12</v>
       </c>
-      <c r="E10" s="37"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
@@ -34903,7 +34933,7 @@
       <c r="D11" s="24">
         <v>12</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
@@ -34937,7 +34967,7 @@
       <c r="D12" s="24">
         <v>12</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
@@ -34971,7 +35001,7 @@
       <c r="D13" s="23">
         <v>12</v>
       </c>
-      <c r="E13" s="38"/>
+      <c r="E13" s="46"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
@@ -35408,10 +35438,10 @@
       <c r="D27">
         <v>8</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="44"/>
       <c r="M27" s="14" t="s">
         <v>300</v>
       </c>
@@ -35437,8 +35467,8 @@
       <c r="D28">
         <v>8</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
       <c r="M28" s="14" t="s">
         <v>298</v>
       </c>
@@ -35464,10 +35494,10 @@
       <c r="D29">
         <v>8</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E29" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="44"/>
       <c r="M29" s="14" t="s">
         <v>295</v>
       </c>
@@ -35493,8 +35523,8 @@
       <c r="D30">
         <v>8</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
       <c r="M30" s="14" t="s">
         <v>293</v>
       </c>
@@ -35520,10 +35550,10 @@
       <c r="D31">
         <v>8</v>
       </c>
-      <c r="E31" s="36" t="s">
+      <c r="E31" s="44" t="s">
         <v>291</v>
       </c>
-      <c r="F31" s="36"/>
+      <c r="F31" s="44"/>
       <c r="M31" s="14" t="s">
         <v>290</v>
       </c>
@@ -35549,8 +35579,8 @@
       <c r="D32">
         <v>8</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
       <c r="M32" s="14" t="s">
         <v>286</v>
       </c>
@@ -35576,10 +35606,10 @@
       <c r="D33">
         <v>8</v>
       </c>
-      <c r="E33" s="36" t="s">
+      <c r="E33" s="44" t="s">
         <v>287</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="44"/>
       <c r="M33" s="14" t="s">
         <v>286</v>
       </c>
@@ -35605,8 +35635,8 @@
       <c r="D34">
         <v>8</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
       <c r="M34" s="14" t="s">
         <v>284</v>
       </c>
@@ -35632,11 +35662,11 @@
       <c r="D35">
         <v>8</v>
       </c>
-      <c r="E35" s="36" t="s">
+      <c r="E35" s="44" t="s">
         <v>282</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
       <c r="H35" s="17" t="s">
         <v>281</v>
       </c>
@@ -35665,9 +35695,9 @@
       <c r="D36">
         <v>8</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
       <c r="M36" s="14" t="s">
         <v>278</v>
       </c>
@@ -36037,7 +36067,7 @@
       <c r="M49" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="N49" s="54" t="s">
+      <c r="N49" s="42" t="s">
         <v>434</v>
       </c>
       <c r="O49">
@@ -36096,7 +36126,7 @@
       <c r="M51" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="N51" s="55" t="s">
+      <c r="N51" s="43" t="s">
         <v>435</v>
       </c>
       <c r="O51">
@@ -36335,843 +36365,843 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="46"/>
-    <col min="2" max="2" width="19.85546875" style="46" customWidth="1"/>
-    <col min="3" max="5" width="29.5703125" style="46" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="46" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" style="46" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="46" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="46" customWidth="1"/>
-    <col min="10" max="257" width="8.7109375" style="46"/>
-    <col min="258" max="258" width="19.85546875" style="46" customWidth="1"/>
-    <col min="259" max="261" width="29.5703125" style="46" customWidth="1"/>
-    <col min="262" max="262" width="22.28515625" style="46" customWidth="1"/>
-    <col min="263" max="263" width="27.5703125" style="46" customWidth="1"/>
-    <col min="264" max="264" width="26.7109375" style="46" customWidth="1"/>
-    <col min="265" max="265" width="20.140625" style="46" customWidth="1"/>
-    <col min="266" max="513" width="8.7109375" style="46"/>
-    <col min="514" max="514" width="19.85546875" style="46" customWidth="1"/>
-    <col min="515" max="517" width="29.5703125" style="46" customWidth="1"/>
-    <col min="518" max="518" width="22.28515625" style="46" customWidth="1"/>
-    <col min="519" max="519" width="27.5703125" style="46" customWidth="1"/>
-    <col min="520" max="520" width="26.7109375" style="46" customWidth="1"/>
-    <col min="521" max="521" width="20.140625" style="46" customWidth="1"/>
-    <col min="522" max="769" width="8.7109375" style="46"/>
-    <col min="770" max="770" width="19.85546875" style="46" customWidth="1"/>
-    <col min="771" max="773" width="29.5703125" style="46" customWidth="1"/>
-    <col min="774" max="774" width="22.28515625" style="46" customWidth="1"/>
-    <col min="775" max="775" width="27.5703125" style="46" customWidth="1"/>
-    <col min="776" max="776" width="26.7109375" style="46" customWidth="1"/>
-    <col min="777" max="777" width="20.140625" style="46" customWidth="1"/>
-    <col min="778" max="1025" width="8.7109375" style="46"/>
-    <col min="1026" max="1026" width="19.85546875" style="46" customWidth="1"/>
-    <col min="1027" max="1029" width="29.5703125" style="46" customWidth="1"/>
-    <col min="1030" max="1030" width="22.28515625" style="46" customWidth="1"/>
-    <col min="1031" max="1031" width="27.5703125" style="46" customWidth="1"/>
-    <col min="1032" max="1032" width="26.7109375" style="46" customWidth="1"/>
-    <col min="1033" max="1033" width="20.140625" style="46" customWidth="1"/>
-    <col min="1034" max="1281" width="8.7109375" style="46"/>
-    <col min="1282" max="1282" width="19.85546875" style="46" customWidth="1"/>
-    <col min="1283" max="1285" width="29.5703125" style="46" customWidth="1"/>
-    <col min="1286" max="1286" width="22.28515625" style="46" customWidth="1"/>
-    <col min="1287" max="1287" width="27.5703125" style="46" customWidth="1"/>
-    <col min="1288" max="1288" width="26.7109375" style="46" customWidth="1"/>
-    <col min="1289" max="1289" width="20.140625" style="46" customWidth="1"/>
-    <col min="1290" max="1537" width="8.7109375" style="46"/>
-    <col min="1538" max="1538" width="19.85546875" style="46" customWidth="1"/>
-    <col min="1539" max="1541" width="29.5703125" style="46" customWidth="1"/>
-    <col min="1542" max="1542" width="22.28515625" style="46" customWidth="1"/>
-    <col min="1543" max="1543" width="27.5703125" style="46" customWidth="1"/>
-    <col min="1544" max="1544" width="26.7109375" style="46" customWidth="1"/>
-    <col min="1545" max="1545" width="20.140625" style="46" customWidth="1"/>
-    <col min="1546" max="1793" width="8.7109375" style="46"/>
-    <col min="1794" max="1794" width="19.85546875" style="46" customWidth="1"/>
-    <col min="1795" max="1797" width="29.5703125" style="46" customWidth="1"/>
-    <col min="1798" max="1798" width="22.28515625" style="46" customWidth="1"/>
-    <col min="1799" max="1799" width="27.5703125" style="46" customWidth="1"/>
-    <col min="1800" max="1800" width="26.7109375" style="46" customWidth="1"/>
-    <col min="1801" max="1801" width="20.140625" style="46" customWidth="1"/>
-    <col min="1802" max="2049" width="8.7109375" style="46"/>
-    <col min="2050" max="2050" width="19.85546875" style="46" customWidth="1"/>
-    <col min="2051" max="2053" width="29.5703125" style="46" customWidth="1"/>
-    <col min="2054" max="2054" width="22.28515625" style="46" customWidth="1"/>
-    <col min="2055" max="2055" width="27.5703125" style="46" customWidth="1"/>
-    <col min="2056" max="2056" width="26.7109375" style="46" customWidth="1"/>
-    <col min="2057" max="2057" width="20.140625" style="46" customWidth="1"/>
-    <col min="2058" max="2305" width="8.7109375" style="46"/>
-    <col min="2306" max="2306" width="19.85546875" style="46" customWidth="1"/>
-    <col min="2307" max="2309" width="29.5703125" style="46" customWidth="1"/>
-    <col min="2310" max="2310" width="22.28515625" style="46" customWidth="1"/>
-    <col min="2311" max="2311" width="27.5703125" style="46" customWidth="1"/>
-    <col min="2312" max="2312" width="26.7109375" style="46" customWidth="1"/>
-    <col min="2313" max="2313" width="20.140625" style="46" customWidth="1"/>
-    <col min="2314" max="2561" width="8.7109375" style="46"/>
-    <col min="2562" max="2562" width="19.85546875" style="46" customWidth="1"/>
-    <col min="2563" max="2565" width="29.5703125" style="46" customWidth="1"/>
-    <col min="2566" max="2566" width="22.28515625" style="46" customWidth="1"/>
-    <col min="2567" max="2567" width="27.5703125" style="46" customWidth="1"/>
-    <col min="2568" max="2568" width="26.7109375" style="46" customWidth="1"/>
-    <col min="2569" max="2569" width="20.140625" style="46" customWidth="1"/>
-    <col min="2570" max="2817" width="8.7109375" style="46"/>
-    <col min="2818" max="2818" width="19.85546875" style="46" customWidth="1"/>
-    <col min="2819" max="2821" width="29.5703125" style="46" customWidth="1"/>
-    <col min="2822" max="2822" width="22.28515625" style="46" customWidth="1"/>
-    <col min="2823" max="2823" width="27.5703125" style="46" customWidth="1"/>
-    <col min="2824" max="2824" width="26.7109375" style="46" customWidth="1"/>
-    <col min="2825" max="2825" width="20.140625" style="46" customWidth="1"/>
-    <col min="2826" max="3073" width="8.7109375" style="46"/>
-    <col min="3074" max="3074" width="19.85546875" style="46" customWidth="1"/>
-    <col min="3075" max="3077" width="29.5703125" style="46" customWidth="1"/>
-    <col min="3078" max="3078" width="22.28515625" style="46" customWidth="1"/>
-    <col min="3079" max="3079" width="27.5703125" style="46" customWidth="1"/>
-    <col min="3080" max="3080" width="26.7109375" style="46" customWidth="1"/>
-    <col min="3081" max="3081" width="20.140625" style="46" customWidth="1"/>
-    <col min="3082" max="3329" width="8.7109375" style="46"/>
-    <col min="3330" max="3330" width="19.85546875" style="46" customWidth="1"/>
-    <col min="3331" max="3333" width="29.5703125" style="46" customWidth="1"/>
-    <col min="3334" max="3334" width="22.28515625" style="46" customWidth="1"/>
-    <col min="3335" max="3335" width="27.5703125" style="46" customWidth="1"/>
-    <col min="3336" max="3336" width="26.7109375" style="46" customWidth="1"/>
-    <col min="3337" max="3337" width="20.140625" style="46" customWidth="1"/>
-    <col min="3338" max="3585" width="8.7109375" style="46"/>
-    <col min="3586" max="3586" width="19.85546875" style="46" customWidth="1"/>
-    <col min="3587" max="3589" width="29.5703125" style="46" customWidth="1"/>
-    <col min="3590" max="3590" width="22.28515625" style="46" customWidth="1"/>
-    <col min="3591" max="3591" width="27.5703125" style="46" customWidth="1"/>
-    <col min="3592" max="3592" width="26.7109375" style="46" customWidth="1"/>
-    <col min="3593" max="3593" width="20.140625" style="46" customWidth="1"/>
-    <col min="3594" max="3841" width="8.7109375" style="46"/>
-    <col min="3842" max="3842" width="19.85546875" style="46" customWidth="1"/>
-    <col min="3843" max="3845" width="29.5703125" style="46" customWidth="1"/>
-    <col min="3846" max="3846" width="22.28515625" style="46" customWidth="1"/>
-    <col min="3847" max="3847" width="27.5703125" style="46" customWidth="1"/>
-    <col min="3848" max="3848" width="26.7109375" style="46" customWidth="1"/>
-    <col min="3849" max="3849" width="20.140625" style="46" customWidth="1"/>
-    <col min="3850" max="4097" width="8.7109375" style="46"/>
-    <col min="4098" max="4098" width="19.85546875" style="46" customWidth="1"/>
-    <col min="4099" max="4101" width="29.5703125" style="46" customWidth="1"/>
-    <col min="4102" max="4102" width="22.28515625" style="46" customWidth="1"/>
-    <col min="4103" max="4103" width="27.5703125" style="46" customWidth="1"/>
-    <col min="4104" max="4104" width="26.7109375" style="46" customWidth="1"/>
-    <col min="4105" max="4105" width="20.140625" style="46" customWidth="1"/>
-    <col min="4106" max="4353" width="8.7109375" style="46"/>
-    <col min="4354" max="4354" width="19.85546875" style="46" customWidth="1"/>
-    <col min="4355" max="4357" width="29.5703125" style="46" customWidth="1"/>
-    <col min="4358" max="4358" width="22.28515625" style="46" customWidth="1"/>
-    <col min="4359" max="4359" width="27.5703125" style="46" customWidth="1"/>
-    <col min="4360" max="4360" width="26.7109375" style="46" customWidth="1"/>
-    <col min="4361" max="4361" width="20.140625" style="46" customWidth="1"/>
-    <col min="4362" max="4609" width="8.7109375" style="46"/>
-    <col min="4610" max="4610" width="19.85546875" style="46" customWidth="1"/>
-    <col min="4611" max="4613" width="29.5703125" style="46" customWidth="1"/>
-    <col min="4614" max="4614" width="22.28515625" style="46" customWidth="1"/>
-    <col min="4615" max="4615" width="27.5703125" style="46" customWidth="1"/>
-    <col min="4616" max="4616" width="26.7109375" style="46" customWidth="1"/>
-    <col min="4617" max="4617" width="20.140625" style="46" customWidth="1"/>
-    <col min="4618" max="4865" width="8.7109375" style="46"/>
-    <col min="4866" max="4866" width="19.85546875" style="46" customWidth="1"/>
-    <col min="4867" max="4869" width="29.5703125" style="46" customWidth="1"/>
-    <col min="4870" max="4870" width="22.28515625" style="46" customWidth="1"/>
-    <col min="4871" max="4871" width="27.5703125" style="46" customWidth="1"/>
-    <col min="4872" max="4872" width="26.7109375" style="46" customWidth="1"/>
-    <col min="4873" max="4873" width="20.140625" style="46" customWidth="1"/>
-    <col min="4874" max="5121" width="8.7109375" style="46"/>
-    <col min="5122" max="5122" width="19.85546875" style="46" customWidth="1"/>
-    <col min="5123" max="5125" width="29.5703125" style="46" customWidth="1"/>
-    <col min="5126" max="5126" width="22.28515625" style="46" customWidth="1"/>
-    <col min="5127" max="5127" width="27.5703125" style="46" customWidth="1"/>
-    <col min="5128" max="5128" width="26.7109375" style="46" customWidth="1"/>
-    <col min="5129" max="5129" width="20.140625" style="46" customWidth="1"/>
-    <col min="5130" max="5377" width="8.7109375" style="46"/>
-    <col min="5378" max="5378" width="19.85546875" style="46" customWidth="1"/>
-    <col min="5379" max="5381" width="29.5703125" style="46" customWidth="1"/>
-    <col min="5382" max="5382" width="22.28515625" style="46" customWidth="1"/>
-    <col min="5383" max="5383" width="27.5703125" style="46" customWidth="1"/>
-    <col min="5384" max="5384" width="26.7109375" style="46" customWidth="1"/>
-    <col min="5385" max="5385" width="20.140625" style="46" customWidth="1"/>
-    <col min="5386" max="5633" width="8.7109375" style="46"/>
-    <col min="5634" max="5634" width="19.85546875" style="46" customWidth="1"/>
-    <col min="5635" max="5637" width="29.5703125" style="46" customWidth="1"/>
-    <col min="5638" max="5638" width="22.28515625" style="46" customWidth="1"/>
-    <col min="5639" max="5639" width="27.5703125" style="46" customWidth="1"/>
-    <col min="5640" max="5640" width="26.7109375" style="46" customWidth="1"/>
-    <col min="5641" max="5641" width="20.140625" style="46" customWidth="1"/>
-    <col min="5642" max="5889" width="8.7109375" style="46"/>
-    <col min="5890" max="5890" width="19.85546875" style="46" customWidth="1"/>
-    <col min="5891" max="5893" width="29.5703125" style="46" customWidth="1"/>
-    <col min="5894" max="5894" width="22.28515625" style="46" customWidth="1"/>
-    <col min="5895" max="5895" width="27.5703125" style="46" customWidth="1"/>
-    <col min="5896" max="5896" width="26.7109375" style="46" customWidth="1"/>
-    <col min="5897" max="5897" width="20.140625" style="46" customWidth="1"/>
-    <col min="5898" max="6145" width="8.7109375" style="46"/>
-    <col min="6146" max="6146" width="19.85546875" style="46" customWidth="1"/>
-    <col min="6147" max="6149" width="29.5703125" style="46" customWidth="1"/>
-    <col min="6150" max="6150" width="22.28515625" style="46" customWidth="1"/>
-    <col min="6151" max="6151" width="27.5703125" style="46" customWidth="1"/>
-    <col min="6152" max="6152" width="26.7109375" style="46" customWidth="1"/>
-    <col min="6153" max="6153" width="20.140625" style="46" customWidth="1"/>
-    <col min="6154" max="6401" width="8.7109375" style="46"/>
-    <col min="6402" max="6402" width="19.85546875" style="46" customWidth="1"/>
-    <col min="6403" max="6405" width="29.5703125" style="46" customWidth="1"/>
-    <col min="6406" max="6406" width="22.28515625" style="46" customWidth="1"/>
-    <col min="6407" max="6407" width="27.5703125" style="46" customWidth="1"/>
-    <col min="6408" max="6408" width="26.7109375" style="46" customWidth="1"/>
-    <col min="6409" max="6409" width="20.140625" style="46" customWidth="1"/>
-    <col min="6410" max="6657" width="8.7109375" style="46"/>
-    <col min="6658" max="6658" width="19.85546875" style="46" customWidth="1"/>
-    <col min="6659" max="6661" width="29.5703125" style="46" customWidth="1"/>
-    <col min="6662" max="6662" width="22.28515625" style="46" customWidth="1"/>
-    <col min="6663" max="6663" width="27.5703125" style="46" customWidth="1"/>
-    <col min="6664" max="6664" width="26.7109375" style="46" customWidth="1"/>
-    <col min="6665" max="6665" width="20.140625" style="46" customWidth="1"/>
-    <col min="6666" max="6913" width="8.7109375" style="46"/>
-    <col min="6914" max="6914" width="19.85546875" style="46" customWidth="1"/>
-    <col min="6915" max="6917" width="29.5703125" style="46" customWidth="1"/>
-    <col min="6918" max="6918" width="22.28515625" style="46" customWidth="1"/>
-    <col min="6919" max="6919" width="27.5703125" style="46" customWidth="1"/>
-    <col min="6920" max="6920" width="26.7109375" style="46" customWidth="1"/>
-    <col min="6921" max="6921" width="20.140625" style="46" customWidth="1"/>
-    <col min="6922" max="7169" width="8.7109375" style="46"/>
-    <col min="7170" max="7170" width="19.85546875" style="46" customWidth="1"/>
-    <col min="7171" max="7173" width="29.5703125" style="46" customWidth="1"/>
-    <col min="7174" max="7174" width="22.28515625" style="46" customWidth="1"/>
-    <col min="7175" max="7175" width="27.5703125" style="46" customWidth="1"/>
-    <col min="7176" max="7176" width="26.7109375" style="46" customWidth="1"/>
-    <col min="7177" max="7177" width="20.140625" style="46" customWidth="1"/>
-    <col min="7178" max="7425" width="8.7109375" style="46"/>
-    <col min="7426" max="7426" width="19.85546875" style="46" customWidth="1"/>
-    <col min="7427" max="7429" width="29.5703125" style="46" customWidth="1"/>
-    <col min="7430" max="7430" width="22.28515625" style="46" customWidth="1"/>
-    <col min="7431" max="7431" width="27.5703125" style="46" customWidth="1"/>
-    <col min="7432" max="7432" width="26.7109375" style="46" customWidth="1"/>
-    <col min="7433" max="7433" width="20.140625" style="46" customWidth="1"/>
-    <col min="7434" max="7681" width="8.7109375" style="46"/>
-    <col min="7682" max="7682" width="19.85546875" style="46" customWidth="1"/>
-    <col min="7683" max="7685" width="29.5703125" style="46" customWidth="1"/>
-    <col min="7686" max="7686" width="22.28515625" style="46" customWidth="1"/>
-    <col min="7687" max="7687" width="27.5703125" style="46" customWidth="1"/>
-    <col min="7688" max="7688" width="26.7109375" style="46" customWidth="1"/>
-    <col min="7689" max="7689" width="20.140625" style="46" customWidth="1"/>
-    <col min="7690" max="7937" width="8.7109375" style="46"/>
-    <col min="7938" max="7938" width="19.85546875" style="46" customWidth="1"/>
-    <col min="7939" max="7941" width="29.5703125" style="46" customWidth="1"/>
-    <col min="7942" max="7942" width="22.28515625" style="46" customWidth="1"/>
-    <col min="7943" max="7943" width="27.5703125" style="46" customWidth="1"/>
-    <col min="7944" max="7944" width="26.7109375" style="46" customWidth="1"/>
-    <col min="7945" max="7945" width="20.140625" style="46" customWidth="1"/>
-    <col min="7946" max="8193" width="8.7109375" style="46"/>
-    <col min="8194" max="8194" width="19.85546875" style="46" customWidth="1"/>
-    <col min="8195" max="8197" width="29.5703125" style="46" customWidth="1"/>
-    <col min="8198" max="8198" width="22.28515625" style="46" customWidth="1"/>
-    <col min="8199" max="8199" width="27.5703125" style="46" customWidth="1"/>
-    <col min="8200" max="8200" width="26.7109375" style="46" customWidth="1"/>
-    <col min="8201" max="8201" width="20.140625" style="46" customWidth="1"/>
-    <col min="8202" max="8449" width="8.7109375" style="46"/>
-    <col min="8450" max="8450" width="19.85546875" style="46" customWidth="1"/>
-    <col min="8451" max="8453" width="29.5703125" style="46" customWidth="1"/>
-    <col min="8454" max="8454" width="22.28515625" style="46" customWidth="1"/>
-    <col min="8455" max="8455" width="27.5703125" style="46" customWidth="1"/>
-    <col min="8456" max="8456" width="26.7109375" style="46" customWidth="1"/>
-    <col min="8457" max="8457" width="20.140625" style="46" customWidth="1"/>
-    <col min="8458" max="8705" width="8.7109375" style="46"/>
-    <col min="8706" max="8706" width="19.85546875" style="46" customWidth="1"/>
-    <col min="8707" max="8709" width="29.5703125" style="46" customWidth="1"/>
-    <col min="8710" max="8710" width="22.28515625" style="46" customWidth="1"/>
-    <col min="8711" max="8711" width="27.5703125" style="46" customWidth="1"/>
-    <col min="8712" max="8712" width="26.7109375" style="46" customWidth="1"/>
-    <col min="8713" max="8713" width="20.140625" style="46" customWidth="1"/>
-    <col min="8714" max="8961" width="8.7109375" style="46"/>
-    <col min="8962" max="8962" width="19.85546875" style="46" customWidth="1"/>
-    <col min="8963" max="8965" width="29.5703125" style="46" customWidth="1"/>
-    <col min="8966" max="8966" width="22.28515625" style="46" customWidth="1"/>
-    <col min="8967" max="8967" width="27.5703125" style="46" customWidth="1"/>
-    <col min="8968" max="8968" width="26.7109375" style="46" customWidth="1"/>
-    <col min="8969" max="8969" width="20.140625" style="46" customWidth="1"/>
-    <col min="8970" max="9217" width="8.7109375" style="46"/>
-    <col min="9218" max="9218" width="19.85546875" style="46" customWidth="1"/>
-    <col min="9219" max="9221" width="29.5703125" style="46" customWidth="1"/>
-    <col min="9222" max="9222" width="22.28515625" style="46" customWidth="1"/>
-    <col min="9223" max="9223" width="27.5703125" style="46" customWidth="1"/>
-    <col min="9224" max="9224" width="26.7109375" style="46" customWidth="1"/>
-    <col min="9225" max="9225" width="20.140625" style="46" customWidth="1"/>
-    <col min="9226" max="9473" width="8.7109375" style="46"/>
-    <col min="9474" max="9474" width="19.85546875" style="46" customWidth="1"/>
-    <col min="9475" max="9477" width="29.5703125" style="46" customWidth="1"/>
-    <col min="9478" max="9478" width="22.28515625" style="46" customWidth="1"/>
-    <col min="9479" max="9479" width="27.5703125" style="46" customWidth="1"/>
-    <col min="9480" max="9480" width="26.7109375" style="46" customWidth="1"/>
-    <col min="9481" max="9481" width="20.140625" style="46" customWidth="1"/>
-    <col min="9482" max="9729" width="8.7109375" style="46"/>
-    <col min="9730" max="9730" width="19.85546875" style="46" customWidth="1"/>
-    <col min="9731" max="9733" width="29.5703125" style="46" customWidth="1"/>
-    <col min="9734" max="9734" width="22.28515625" style="46" customWidth="1"/>
-    <col min="9735" max="9735" width="27.5703125" style="46" customWidth="1"/>
-    <col min="9736" max="9736" width="26.7109375" style="46" customWidth="1"/>
-    <col min="9737" max="9737" width="20.140625" style="46" customWidth="1"/>
-    <col min="9738" max="9985" width="8.7109375" style="46"/>
-    <col min="9986" max="9986" width="19.85546875" style="46" customWidth="1"/>
-    <col min="9987" max="9989" width="29.5703125" style="46" customWidth="1"/>
-    <col min="9990" max="9990" width="22.28515625" style="46" customWidth="1"/>
-    <col min="9991" max="9991" width="27.5703125" style="46" customWidth="1"/>
-    <col min="9992" max="9992" width="26.7109375" style="46" customWidth="1"/>
-    <col min="9993" max="9993" width="20.140625" style="46" customWidth="1"/>
-    <col min="9994" max="10241" width="8.7109375" style="46"/>
-    <col min="10242" max="10242" width="19.85546875" style="46" customWidth="1"/>
-    <col min="10243" max="10245" width="29.5703125" style="46" customWidth="1"/>
-    <col min="10246" max="10246" width="22.28515625" style="46" customWidth="1"/>
-    <col min="10247" max="10247" width="27.5703125" style="46" customWidth="1"/>
-    <col min="10248" max="10248" width="26.7109375" style="46" customWidth="1"/>
-    <col min="10249" max="10249" width="20.140625" style="46" customWidth="1"/>
-    <col min="10250" max="10497" width="8.7109375" style="46"/>
-    <col min="10498" max="10498" width="19.85546875" style="46" customWidth="1"/>
-    <col min="10499" max="10501" width="29.5703125" style="46" customWidth="1"/>
-    <col min="10502" max="10502" width="22.28515625" style="46" customWidth="1"/>
-    <col min="10503" max="10503" width="27.5703125" style="46" customWidth="1"/>
-    <col min="10504" max="10504" width="26.7109375" style="46" customWidth="1"/>
-    <col min="10505" max="10505" width="20.140625" style="46" customWidth="1"/>
-    <col min="10506" max="10753" width="8.7109375" style="46"/>
-    <col min="10754" max="10754" width="19.85546875" style="46" customWidth="1"/>
-    <col min="10755" max="10757" width="29.5703125" style="46" customWidth="1"/>
-    <col min="10758" max="10758" width="22.28515625" style="46" customWidth="1"/>
-    <col min="10759" max="10759" width="27.5703125" style="46" customWidth="1"/>
-    <col min="10760" max="10760" width="26.7109375" style="46" customWidth="1"/>
-    <col min="10761" max="10761" width="20.140625" style="46" customWidth="1"/>
-    <col min="10762" max="11009" width="8.7109375" style="46"/>
-    <col min="11010" max="11010" width="19.85546875" style="46" customWidth="1"/>
-    <col min="11011" max="11013" width="29.5703125" style="46" customWidth="1"/>
-    <col min="11014" max="11014" width="22.28515625" style="46" customWidth="1"/>
-    <col min="11015" max="11015" width="27.5703125" style="46" customWidth="1"/>
-    <col min="11016" max="11016" width="26.7109375" style="46" customWidth="1"/>
-    <col min="11017" max="11017" width="20.140625" style="46" customWidth="1"/>
-    <col min="11018" max="11265" width="8.7109375" style="46"/>
-    <col min="11266" max="11266" width="19.85546875" style="46" customWidth="1"/>
-    <col min="11267" max="11269" width="29.5703125" style="46" customWidth="1"/>
-    <col min="11270" max="11270" width="22.28515625" style="46" customWidth="1"/>
-    <col min="11271" max="11271" width="27.5703125" style="46" customWidth="1"/>
-    <col min="11272" max="11272" width="26.7109375" style="46" customWidth="1"/>
-    <col min="11273" max="11273" width="20.140625" style="46" customWidth="1"/>
-    <col min="11274" max="11521" width="8.7109375" style="46"/>
-    <col min="11522" max="11522" width="19.85546875" style="46" customWidth="1"/>
-    <col min="11523" max="11525" width="29.5703125" style="46" customWidth="1"/>
-    <col min="11526" max="11526" width="22.28515625" style="46" customWidth="1"/>
-    <col min="11527" max="11527" width="27.5703125" style="46" customWidth="1"/>
-    <col min="11528" max="11528" width="26.7109375" style="46" customWidth="1"/>
-    <col min="11529" max="11529" width="20.140625" style="46" customWidth="1"/>
-    <col min="11530" max="11777" width="8.7109375" style="46"/>
-    <col min="11778" max="11778" width="19.85546875" style="46" customWidth="1"/>
-    <col min="11779" max="11781" width="29.5703125" style="46" customWidth="1"/>
-    <col min="11782" max="11782" width="22.28515625" style="46" customWidth="1"/>
-    <col min="11783" max="11783" width="27.5703125" style="46" customWidth="1"/>
-    <col min="11784" max="11784" width="26.7109375" style="46" customWidth="1"/>
-    <col min="11785" max="11785" width="20.140625" style="46" customWidth="1"/>
-    <col min="11786" max="12033" width="8.7109375" style="46"/>
-    <col min="12034" max="12034" width="19.85546875" style="46" customWidth="1"/>
-    <col min="12035" max="12037" width="29.5703125" style="46" customWidth="1"/>
-    <col min="12038" max="12038" width="22.28515625" style="46" customWidth="1"/>
-    <col min="12039" max="12039" width="27.5703125" style="46" customWidth="1"/>
-    <col min="12040" max="12040" width="26.7109375" style="46" customWidth="1"/>
-    <col min="12041" max="12041" width="20.140625" style="46" customWidth="1"/>
-    <col min="12042" max="12289" width="8.7109375" style="46"/>
-    <col min="12290" max="12290" width="19.85546875" style="46" customWidth="1"/>
-    <col min="12291" max="12293" width="29.5703125" style="46" customWidth="1"/>
-    <col min="12294" max="12294" width="22.28515625" style="46" customWidth="1"/>
-    <col min="12295" max="12295" width="27.5703125" style="46" customWidth="1"/>
-    <col min="12296" max="12296" width="26.7109375" style="46" customWidth="1"/>
-    <col min="12297" max="12297" width="20.140625" style="46" customWidth="1"/>
-    <col min="12298" max="12545" width="8.7109375" style="46"/>
-    <col min="12546" max="12546" width="19.85546875" style="46" customWidth="1"/>
-    <col min="12547" max="12549" width="29.5703125" style="46" customWidth="1"/>
-    <col min="12550" max="12550" width="22.28515625" style="46" customWidth="1"/>
-    <col min="12551" max="12551" width="27.5703125" style="46" customWidth="1"/>
-    <col min="12552" max="12552" width="26.7109375" style="46" customWidth="1"/>
-    <col min="12553" max="12553" width="20.140625" style="46" customWidth="1"/>
-    <col min="12554" max="12801" width="8.7109375" style="46"/>
-    <col min="12802" max="12802" width="19.85546875" style="46" customWidth="1"/>
-    <col min="12803" max="12805" width="29.5703125" style="46" customWidth="1"/>
-    <col min="12806" max="12806" width="22.28515625" style="46" customWidth="1"/>
-    <col min="12807" max="12807" width="27.5703125" style="46" customWidth="1"/>
-    <col min="12808" max="12808" width="26.7109375" style="46" customWidth="1"/>
-    <col min="12809" max="12809" width="20.140625" style="46" customWidth="1"/>
-    <col min="12810" max="13057" width="8.7109375" style="46"/>
-    <col min="13058" max="13058" width="19.85546875" style="46" customWidth="1"/>
-    <col min="13059" max="13061" width="29.5703125" style="46" customWidth="1"/>
-    <col min="13062" max="13062" width="22.28515625" style="46" customWidth="1"/>
-    <col min="13063" max="13063" width="27.5703125" style="46" customWidth="1"/>
-    <col min="13064" max="13064" width="26.7109375" style="46" customWidth="1"/>
-    <col min="13065" max="13065" width="20.140625" style="46" customWidth="1"/>
-    <col min="13066" max="13313" width="8.7109375" style="46"/>
-    <col min="13314" max="13314" width="19.85546875" style="46" customWidth="1"/>
-    <col min="13315" max="13317" width="29.5703125" style="46" customWidth="1"/>
-    <col min="13318" max="13318" width="22.28515625" style="46" customWidth="1"/>
-    <col min="13319" max="13319" width="27.5703125" style="46" customWidth="1"/>
-    <col min="13320" max="13320" width="26.7109375" style="46" customWidth="1"/>
-    <col min="13321" max="13321" width="20.140625" style="46" customWidth="1"/>
-    <col min="13322" max="13569" width="8.7109375" style="46"/>
-    <col min="13570" max="13570" width="19.85546875" style="46" customWidth="1"/>
-    <col min="13571" max="13573" width="29.5703125" style="46" customWidth="1"/>
-    <col min="13574" max="13574" width="22.28515625" style="46" customWidth="1"/>
-    <col min="13575" max="13575" width="27.5703125" style="46" customWidth="1"/>
-    <col min="13576" max="13576" width="26.7109375" style="46" customWidth="1"/>
-    <col min="13577" max="13577" width="20.140625" style="46" customWidth="1"/>
-    <col min="13578" max="13825" width="8.7109375" style="46"/>
-    <col min="13826" max="13826" width="19.85546875" style="46" customWidth="1"/>
-    <col min="13827" max="13829" width="29.5703125" style="46" customWidth="1"/>
-    <col min="13830" max="13830" width="22.28515625" style="46" customWidth="1"/>
-    <col min="13831" max="13831" width="27.5703125" style="46" customWidth="1"/>
-    <col min="13832" max="13832" width="26.7109375" style="46" customWidth="1"/>
-    <col min="13833" max="13833" width="20.140625" style="46" customWidth="1"/>
-    <col min="13834" max="14081" width="8.7109375" style="46"/>
-    <col min="14082" max="14082" width="19.85546875" style="46" customWidth="1"/>
-    <col min="14083" max="14085" width="29.5703125" style="46" customWidth="1"/>
-    <col min="14086" max="14086" width="22.28515625" style="46" customWidth="1"/>
-    <col min="14087" max="14087" width="27.5703125" style="46" customWidth="1"/>
-    <col min="14088" max="14088" width="26.7109375" style="46" customWidth="1"/>
-    <col min="14089" max="14089" width="20.140625" style="46" customWidth="1"/>
-    <col min="14090" max="14337" width="8.7109375" style="46"/>
-    <col min="14338" max="14338" width="19.85546875" style="46" customWidth="1"/>
-    <col min="14339" max="14341" width="29.5703125" style="46" customWidth="1"/>
-    <col min="14342" max="14342" width="22.28515625" style="46" customWidth="1"/>
-    <col min="14343" max="14343" width="27.5703125" style="46" customWidth="1"/>
-    <col min="14344" max="14344" width="26.7109375" style="46" customWidth="1"/>
-    <col min="14345" max="14345" width="20.140625" style="46" customWidth="1"/>
-    <col min="14346" max="14593" width="8.7109375" style="46"/>
-    <col min="14594" max="14594" width="19.85546875" style="46" customWidth="1"/>
-    <col min="14595" max="14597" width="29.5703125" style="46" customWidth="1"/>
-    <col min="14598" max="14598" width="22.28515625" style="46" customWidth="1"/>
-    <col min="14599" max="14599" width="27.5703125" style="46" customWidth="1"/>
-    <col min="14600" max="14600" width="26.7109375" style="46" customWidth="1"/>
-    <col min="14601" max="14601" width="20.140625" style="46" customWidth="1"/>
-    <col min="14602" max="14849" width="8.7109375" style="46"/>
-    <col min="14850" max="14850" width="19.85546875" style="46" customWidth="1"/>
-    <col min="14851" max="14853" width="29.5703125" style="46" customWidth="1"/>
-    <col min="14854" max="14854" width="22.28515625" style="46" customWidth="1"/>
-    <col min="14855" max="14855" width="27.5703125" style="46" customWidth="1"/>
-    <col min="14856" max="14856" width="26.7109375" style="46" customWidth="1"/>
-    <col min="14857" max="14857" width="20.140625" style="46" customWidth="1"/>
-    <col min="14858" max="15105" width="8.7109375" style="46"/>
-    <col min="15106" max="15106" width="19.85546875" style="46" customWidth="1"/>
-    <col min="15107" max="15109" width="29.5703125" style="46" customWidth="1"/>
-    <col min="15110" max="15110" width="22.28515625" style="46" customWidth="1"/>
-    <col min="15111" max="15111" width="27.5703125" style="46" customWidth="1"/>
-    <col min="15112" max="15112" width="26.7109375" style="46" customWidth="1"/>
-    <col min="15113" max="15113" width="20.140625" style="46" customWidth="1"/>
-    <col min="15114" max="15361" width="8.7109375" style="46"/>
-    <col min="15362" max="15362" width="19.85546875" style="46" customWidth="1"/>
-    <col min="15363" max="15365" width="29.5703125" style="46" customWidth="1"/>
-    <col min="15366" max="15366" width="22.28515625" style="46" customWidth="1"/>
-    <col min="15367" max="15367" width="27.5703125" style="46" customWidth="1"/>
-    <col min="15368" max="15368" width="26.7109375" style="46" customWidth="1"/>
-    <col min="15369" max="15369" width="20.140625" style="46" customWidth="1"/>
-    <col min="15370" max="15617" width="8.7109375" style="46"/>
-    <col min="15618" max="15618" width="19.85546875" style="46" customWidth="1"/>
-    <col min="15619" max="15621" width="29.5703125" style="46" customWidth="1"/>
-    <col min="15622" max="15622" width="22.28515625" style="46" customWidth="1"/>
-    <col min="15623" max="15623" width="27.5703125" style="46" customWidth="1"/>
-    <col min="15624" max="15624" width="26.7109375" style="46" customWidth="1"/>
-    <col min="15625" max="15625" width="20.140625" style="46" customWidth="1"/>
-    <col min="15626" max="15873" width="8.7109375" style="46"/>
-    <col min="15874" max="15874" width="19.85546875" style="46" customWidth="1"/>
-    <col min="15875" max="15877" width="29.5703125" style="46" customWidth="1"/>
-    <col min="15878" max="15878" width="22.28515625" style="46" customWidth="1"/>
-    <col min="15879" max="15879" width="27.5703125" style="46" customWidth="1"/>
-    <col min="15880" max="15880" width="26.7109375" style="46" customWidth="1"/>
-    <col min="15881" max="15881" width="20.140625" style="46" customWidth="1"/>
-    <col min="15882" max="16129" width="8.7109375" style="46"/>
-    <col min="16130" max="16130" width="19.85546875" style="46" customWidth="1"/>
-    <col min="16131" max="16133" width="29.5703125" style="46" customWidth="1"/>
-    <col min="16134" max="16134" width="22.28515625" style="46" customWidth="1"/>
-    <col min="16135" max="16135" width="27.5703125" style="46" customWidth="1"/>
-    <col min="16136" max="16136" width="26.7109375" style="46" customWidth="1"/>
-    <col min="16137" max="16137" width="20.140625" style="46" customWidth="1"/>
-    <col min="16138" max="16384" width="8.7109375" style="46"/>
+    <col min="1" max="1" width="8.7109375" style="36"/>
+    <col min="2" max="2" width="19.85546875" style="36" customWidth="1"/>
+    <col min="3" max="5" width="29.5703125" style="36" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" style="36" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="36" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="36" customWidth="1"/>
+    <col min="10" max="257" width="8.7109375" style="36"/>
+    <col min="258" max="258" width="19.85546875" style="36" customWidth="1"/>
+    <col min="259" max="261" width="29.5703125" style="36" customWidth="1"/>
+    <col min="262" max="262" width="22.28515625" style="36" customWidth="1"/>
+    <col min="263" max="263" width="27.5703125" style="36" customWidth="1"/>
+    <col min="264" max="264" width="26.7109375" style="36" customWidth="1"/>
+    <col min="265" max="265" width="20.140625" style="36" customWidth="1"/>
+    <col min="266" max="513" width="8.7109375" style="36"/>
+    <col min="514" max="514" width="19.85546875" style="36" customWidth="1"/>
+    <col min="515" max="517" width="29.5703125" style="36" customWidth="1"/>
+    <col min="518" max="518" width="22.28515625" style="36" customWidth="1"/>
+    <col min="519" max="519" width="27.5703125" style="36" customWidth="1"/>
+    <col min="520" max="520" width="26.7109375" style="36" customWidth="1"/>
+    <col min="521" max="521" width="20.140625" style="36" customWidth="1"/>
+    <col min="522" max="769" width="8.7109375" style="36"/>
+    <col min="770" max="770" width="19.85546875" style="36" customWidth="1"/>
+    <col min="771" max="773" width="29.5703125" style="36" customWidth="1"/>
+    <col min="774" max="774" width="22.28515625" style="36" customWidth="1"/>
+    <col min="775" max="775" width="27.5703125" style="36" customWidth="1"/>
+    <col min="776" max="776" width="26.7109375" style="36" customWidth="1"/>
+    <col min="777" max="777" width="20.140625" style="36" customWidth="1"/>
+    <col min="778" max="1025" width="8.7109375" style="36"/>
+    <col min="1026" max="1026" width="19.85546875" style="36" customWidth="1"/>
+    <col min="1027" max="1029" width="29.5703125" style="36" customWidth="1"/>
+    <col min="1030" max="1030" width="22.28515625" style="36" customWidth="1"/>
+    <col min="1031" max="1031" width="27.5703125" style="36" customWidth="1"/>
+    <col min="1032" max="1032" width="26.7109375" style="36" customWidth="1"/>
+    <col min="1033" max="1033" width="20.140625" style="36" customWidth="1"/>
+    <col min="1034" max="1281" width="8.7109375" style="36"/>
+    <col min="1282" max="1282" width="19.85546875" style="36" customWidth="1"/>
+    <col min="1283" max="1285" width="29.5703125" style="36" customWidth="1"/>
+    <col min="1286" max="1286" width="22.28515625" style="36" customWidth="1"/>
+    <col min="1287" max="1287" width="27.5703125" style="36" customWidth="1"/>
+    <col min="1288" max="1288" width="26.7109375" style="36" customWidth="1"/>
+    <col min="1289" max="1289" width="20.140625" style="36" customWidth="1"/>
+    <col min="1290" max="1537" width="8.7109375" style="36"/>
+    <col min="1538" max="1538" width="19.85546875" style="36" customWidth="1"/>
+    <col min="1539" max="1541" width="29.5703125" style="36" customWidth="1"/>
+    <col min="1542" max="1542" width="22.28515625" style="36" customWidth="1"/>
+    <col min="1543" max="1543" width="27.5703125" style="36" customWidth="1"/>
+    <col min="1544" max="1544" width="26.7109375" style="36" customWidth="1"/>
+    <col min="1545" max="1545" width="20.140625" style="36" customWidth="1"/>
+    <col min="1546" max="1793" width="8.7109375" style="36"/>
+    <col min="1794" max="1794" width="19.85546875" style="36" customWidth="1"/>
+    <col min="1795" max="1797" width="29.5703125" style="36" customWidth="1"/>
+    <col min="1798" max="1798" width="22.28515625" style="36" customWidth="1"/>
+    <col min="1799" max="1799" width="27.5703125" style="36" customWidth="1"/>
+    <col min="1800" max="1800" width="26.7109375" style="36" customWidth="1"/>
+    <col min="1801" max="1801" width="20.140625" style="36" customWidth="1"/>
+    <col min="1802" max="2049" width="8.7109375" style="36"/>
+    <col min="2050" max="2050" width="19.85546875" style="36" customWidth="1"/>
+    <col min="2051" max="2053" width="29.5703125" style="36" customWidth="1"/>
+    <col min="2054" max="2054" width="22.28515625" style="36" customWidth="1"/>
+    <col min="2055" max="2055" width="27.5703125" style="36" customWidth="1"/>
+    <col min="2056" max="2056" width="26.7109375" style="36" customWidth="1"/>
+    <col min="2057" max="2057" width="20.140625" style="36" customWidth="1"/>
+    <col min="2058" max="2305" width="8.7109375" style="36"/>
+    <col min="2306" max="2306" width="19.85546875" style="36" customWidth="1"/>
+    <col min="2307" max="2309" width="29.5703125" style="36" customWidth="1"/>
+    <col min="2310" max="2310" width="22.28515625" style="36" customWidth="1"/>
+    <col min="2311" max="2311" width="27.5703125" style="36" customWidth="1"/>
+    <col min="2312" max="2312" width="26.7109375" style="36" customWidth="1"/>
+    <col min="2313" max="2313" width="20.140625" style="36" customWidth="1"/>
+    <col min="2314" max="2561" width="8.7109375" style="36"/>
+    <col min="2562" max="2562" width="19.85546875" style="36" customWidth="1"/>
+    <col min="2563" max="2565" width="29.5703125" style="36" customWidth="1"/>
+    <col min="2566" max="2566" width="22.28515625" style="36" customWidth="1"/>
+    <col min="2567" max="2567" width="27.5703125" style="36" customWidth="1"/>
+    <col min="2568" max="2568" width="26.7109375" style="36" customWidth="1"/>
+    <col min="2569" max="2569" width="20.140625" style="36" customWidth="1"/>
+    <col min="2570" max="2817" width="8.7109375" style="36"/>
+    <col min="2818" max="2818" width="19.85546875" style="36" customWidth="1"/>
+    <col min="2819" max="2821" width="29.5703125" style="36" customWidth="1"/>
+    <col min="2822" max="2822" width="22.28515625" style="36" customWidth="1"/>
+    <col min="2823" max="2823" width="27.5703125" style="36" customWidth="1"/>
+    <col min="2824" max="2824" width="26.7109375" style="36" customWidth="1"/>
+    <col min="2825" max="2825" width="20.140625" style="36" customWidth="1"/>
+    <col min="2826" max="3073" width="8.7109375" style="36"/>
+    <col min="3074" max="3074" width="19.85546875" style="36" customWidth="1"/>
+    <col min="3075" max="3077" width="29.5703125" style="36" customWidth="1"/>
+    <col min="3078" max="3078" width="22.28515625" style="36" customWidth="1"/>
+    <col min="3079" max="3079" width="27.5703125" style="36" customWidth="1"/>
+    <col min="3080" max="3080" width="26.7109375" style="36" customWidth="1"/>
+    <col min="3081" max="3081" width="20.140625" style="36" customWidth="1"/>
+    <col min="3082" max="3329" width="8.7109375" style="36"/>
+    <col min="3330" max="3330" width="19.85546875" style="36" customWidth="1"/>
+    <col min="3331" max="3333" width="29.5703125" style="36" customWidth="1"/>
+    <col min="3334" max="3334" width="22.28515625" style="36" customWidth="1"/>
+    <col min="3335" max="3335" width="27.5703125" style="36" customWidth="1"/>
+    <col min="3336" max="3336" width="26.7109375" style="36" customWidth="1"/>
+    <col min="3337" max="3337" width="20.140625" style="36" customWidth="1"/>
+    <col min="3338" max="3585" width="8.7109375" style="36"/>
+    <col min="3586" max="3586" width="19.85546875" style="36" customWidth="1"/>
+    <col min="3587" max="3589" width="29.5703125" style="36" customWidth="1"/>
+    <col min="3590" max="3590" width="22.28515625" style="36" customWidth="1"/>
+    <col min="3591" max="3591" width="27.5703125" style="36" customWidth="1"/>
+    <col min="3592" max="3592" width="26.7109375" style="36" customWidth="1"/>
+    <col min="3593" max="3593" width="20.140625" style="36" customWidth="1"/>
+    <col min="3594" max="3841" width="8.7109375" style="36"/>
+    <col min="3842" max="3842" width="19.85546875" style="36" customWidth="1"/>
+    <col min="3843" max="3845" width="29.5703125" style="36" customWidth="1"/>
+    <col min="3846" max="3846" width="22.28515625" style="36" customWidth="1"/>
+    <col min="3847" max="3847" width="27.5703125" style="36" customWidth="1"/>
+    <col min="3848" max="3848" width="26.7109375" style="36" customWidth="1"/>
+    <col min="3849" max="3849" width="20.140625" style="36" customWidth="1"/>
+    <col min="3850" max="4097" width="8.7109375" style="36"/>
+    <col min="4098" max="4098" width="19.85546875" style="36" customWidth="1"/>
+    <col min="4099" max="4101" width="29.5703125" style="36" customWidth="1"/>
+    <col min="4102" max="4102" width="22.28515625" style="36" customWidth="1"/>
+    <col min="4103" max="4103" width="27.5703125" style="36" customWidth="1"/>
+    <col min="4104" max="4104" width="26.7109375" style="36" customWidth="1"/>
+    <col min="4105" max="4105" width="20.140625" style="36" customWidth="1"/>
+    <col min="4106" max="4353" width="8.7109375" style="36"/>
+    <col min="4354" max="4354" width="19.85546875" style="36" customWidth="1"/>
+    <col min="4355" max="4357" width="29.5703125" style="36" customWidth="1"/>
+    <col min="4358" max="4358" width="22.28515625" style="36" customWidth="1"/>
+    <col min="4359" max="4359" width="27.5703125" style="36" customWidth="1"/>
+    <col min="4360" max="4360" width="26.7109375" style="36" customWidth="1"/>
+    <col min="4361" max="4361" width="20.140625" style="36" customWidth="1"/>
+    <col min="4362" max="4609" width="8.7109375" style="36"/>
+    <col min="4610" max="4610" width="19.85546875" style="36" customWidth="1"/>
+    <col min="4611" max="4613" width="29.5703125" style="36" customWidth="1"/>
+    <col min="4614" max="4614" width="22.28515625" style="36" customWidth="1"/>
+    <col min="4615" max="4615" width="27.5703125" style="36" customWidth="1"/>
+    <col min="4616" max="4616" width="26.7109375" style="36" customWidth="1"/>
+    <col min="4617" max="4617" width="20.140625" style="36" customWidth="1"/>
+    <col min="4618" max="4865" width="8.7109375" style="36"/>
+    <col min="4866" max="4866" width="19.85546875" style="36" customWidth="1"/>
+    <col min="4867" max="4869" width="29.5703125" style="36" customWidth="1"/>
+    <col min="4870" max="4870" width="22.28515625" style="36" customWidth="1"/>
+    <col min="4871" max="4871" width="27.5703125" style="36" customWidth="1"/>
+    <col min="4872" max="4872" width="26.7109375" style="36" customWidth="1"/>
+    <col min="4873" max="4873" width="20.140625" style="36" customWidth="1"/>
+    <col min="4874" max="5121" width="8.7109375" style="36"/>
+    <col min="5122" max="5122" width="19.85546875" style="36" customWidth="1"/>
+    <col min="5123" max="5125" width="29.5703125" style="36" customWidth="1"/>
+    <col min="5126" max="5126" width="22.28515625" style="36" customWidth="1"/>
+    <col min="5127" max="5127" width="27.5703125" style="36" customWidth="1"/>
+    <col min="5128" max="5128" width="26.7109375" style="36" customWidth="1"/>
+    <col min="5129" max="5129" width="20.140625" style="36" customWidth="1"/>
+    <col min="5130" max="5377" width="8.7109375" style="36"/>
+    <col min="5378" max="5378" width="19.85546875" style="36" customWidth="1"/>
+    <col min="5379" max="5381" width="29.5703125" style="36" customWidth="1"/>
+    <col min="5382" max="5382" width="22.28515625" style="36" customWidth="1"/>
+    <col min="5383" max="5383" width="27.5703125" style="36" customWidth="1"/>
+    <col min="5384" max="5384" width="26.7109375" style="36" customWidth="1"/>
+    <col min="5385" max="5385" width="20.140625" style="36" customWidth="1"/>
+    <col min="5386" max="5633" width="8.7109375" style="36"/>
+    <col min="5634" max="5634" width="19.85546875" style="36" customWidth="1"/>
+    <col min="5635" max="5637" width="29.5703125" style="36" customWidth="1"/>
+    <col min="5638" max="5638" width="22.28515625" style="36" customWidth="1"/>
+    <col min="5639" max="5639" width="27.5703125" style="36" customWidth="1"/>
+    <col min="5640" max="5640" width="26.7109375" style="36" customWidth="1"/>
+    <col min="5641" max="5641" width="20.140625" style="36" customWidth="1"/>
+    <col min="5642" max="5889" width="8.7109375" style="36"/>
+    <col min="5890" max="5890" width="19.85546875" style="36" customWidth="1"/>
+    <col min="5891" max="5893" width="29.5703125" style="36" customWidth="1"/>
+    <col min="5894" max="5894" width="22.28515625" style="36" customWidth="1"/>
+    <col min="5895" max="5895" width="27.5703125" style="36" customWidth="1"/>
+    <col min="5896" max="5896" width="26.7109375" style="36" customWidth="1"/>
+    <col min="5897" max="5897" width="20.140625" style="36" customWidth="1"/>
+    <col min="5898" max="6145" width="8.7109375" style="36"/>
+    <col min="6146" max="6146" width="19.85546875" style="36" customWidth="1"/>
+    <col min="6147" max="6149" width="29.5703125" style="36" customWidth="1"/>
+    <col min="6150" max="6150" width="22.28515625" style="36" customWidth="1"/>
+    <col min="6151" max="6151" width="27.5703125" style="36" customWidth="1"/>
+    <col min="6152" max="6152" width="26.7109375" style="36" customWidth="1"/>
+    <col min="6153" max="6153" width="20.140625" style="36" customWidth="1"/>
+    <col min="6154" max="6401" width="8.7109375" style="36"/>
+    <col min="6402" max="6402" width="19.85546875" style="36" customWidth="1"/>
+    <col min="6403" max="6405" width="29.5703125" style="36" customWidth="1"/>
+    <col min="6406" max="6406" width="22.28515625" style="36" customWidth="1"/>
+    <col min="6407" max="6407" width="27.5703125" style="36" customWidth="1"/>
+    <col min="6408" max="6408" width="26.7109375" style="36" customWidth="1"/>
+    <col min="6409" max="6409" width="20.140625" style="36" customWidth="1"/>
+    <col min="6410" max="6657" width="8.7109375" style="36"/>
+    <col min="6658" max="6658" width="19.85546875" style="36" customWidth="1"/>
+    <col min="6659" max="6661" width="29.5703125" style="36" customWidth="1"/>
+    <col min="6662" max="6662" width="22.28515625" style="36" customWidth="1"/>
+    <col min="6663" max="6663" width="27.5703125" style="36" customWidth="1"/>
+    <col min="6664" max="6664" width="26.7109375" style="36" customWidth="1"/>
+    <col min="6665" max="6665" width="20.140625" style="36" customWidth="1"/>
+    <col min="6666" max="6913" width="8.7109375" style="36"/>
+    <col min="6914" max="6914" width="19.85546875" style="36" customWidth="1"/>
+    <col min="6915" max="6917" width="29.5703125" style="36" customWidth="1"/>
+    <col min="6918" max="6918" width="22.28515625" style="36" customWidth="1"/>
+    <col min="6919" max="6919" width="27.5703125" style="36" customWidth="1"/>
+    <col min="6920" max="6920" width="26.7109375" style="36" customWidth="1"/>
+    <col min="6921" max="6921" width="20.140625" style="36" customWidth="1"/>
+    <col min="6922" max="7169" width="8.7109375" style="36"/>
+    <col min="7170" max="7170" width="19.85546875" style="36" customWidth="1"/>
+    <col min="7171" max="7173" width="29.5703125" style="36" customWidth="1"/>
+    <col min="7174" max="7174" width="22.28515625" style="36" customWidth="1"/>
+    <col min="7175" max="7175" width="27.5703125" style="36" customWidth="1"/>
+    <col min="7176" max="7176" width="26.7109375" style="36" customWidth="1"/>
+    <col min="7177" max="7177" width="20.140625" style="36" customWidth="1"/>
+    <col min="7178" max="7425" width="8.7109375" style="36"/>
+    <col min="7426" max="7426" width="19.85546875" style="36" customWidth="1"/>
+    <col min="7427" max="7429" width="29.5703125" style="36" customWidth="1"/>
+    <col min="7430" max="7430" width="22.28515625" style="36" customWidth="1"/>
+    <col min="7431" max="7431" width="27.5703125" style="36" customWidth="1"/>
+    <col min="7432" max="7432" width="26.7109375" style="36" customWidth="1"/>
+    <col min="7433" max="7433" width="20.140625" style="36" customWidth="1"/>
+    <col min="7434" max="7681" width="8.7109375" style="36"/>
+    <col min="7682" max="7682" width="19.85546875" style="36" customWidth="1"/>
+    <col min="7683" max="7685" width="29.5703125" style="36" customWidth="1"/>
+    <col min="7686" max="7686" width="22.28515625" style="36" customWidth="1"/>
+    <col min="7687" max="7687" width="27.5703125" style="36" customWidth="1"/>
+    <col min="7688" max="7688" width="26.7109375" style="36" customWidth="1"/>
+    <col min="7689" max="7689" width="20.140625" style="36" customWidth="1"/>
+    <col min="7690" max="7937" width="8.7109375" style="36"/>
+    <col min="7938" max="7938" width="19.85546875" style="36" customWidth="1"/>
+    <col min="7939" max="7941" width="29.5703125" style="36" customWidth="1"/>
+    <col min="7942" max="7942" width="22.28515625" style="36" customWidth="1"/>
+    <col min="7943" max="7943" width="27.5703125" style="36" customWidth="1"/>
+    <col min="7944" max="7944" width="26.7109375" style="36" customWidth="1"/>
+    <col min="7945" max="7945" width="20.140625" style="36" customWidth="1"/>
+    <col min="7946" max="8193" width="8.7109375" style="36"/>
+    <col min="8194" max="8194" width="19.85546875" style="36" customWidth="1"/>
+    <col min="8195" max="8197" width="29.5703125" style="36" customWidth="1"/>
+    <col min="8198" max="8198" width="22.28515625" style="36" customWidth="1"/>
+    <col min="8199" max="8199" width="27.5703125" style="36" customWidth="1"/>
+    <col min="8200" max="8200" width="26.7109375" style="36" customWidth="1"/>
+    <col min="8201" max="8201" width="20.140625" style="36" customWidth="1"/>
+    <col min="8202" max="8449" width="8.7109375" style="36"/>
+    <col min="8450" max="8450" width="19.85546875" style="36" customWidth="1"/>
+    <col min="8451" max="8453" width="29.5703125" style="36" customWidth="1"/>
+    <col min="8454" max="8454" width="22.28515625" style="36" customWidth="1"/>
+    <col min="8455" max="8455" width="27.5703125" style="36" customWidth="1"/>
+    <col min="8456" max="8456" width="26.7109375" style="36" customWidth="1"/>
+    <col min="8457" max="8457" width="20.140625" style="36" customWidth="1"/>
+    <col min="8458" max="8705" width="8.7109375" style="36"/>
+    <col min="8706" max="8706" width="19.85546875" style="36" customWidth="1"/>
+    <col min="8707" max="8709" width="29.5703125" style="36" customWidth="1"/>
+    <col min="8710" max="8710" width="22.28515625" style="36" customWidth="1"/>
+    <col min="8711" max="8711" width="27.5703125" style="36" customWidth="1"/>
+    <col min="8712" max="8712" width="26.7109375" style="36" customWidth="1"/>
+    <col min="8713" max="8713" width="20.140625" style="36" customWidth="1"/>
+    <col min="8714" max="8961" width="8.7109375" style="36"/>
+    <col min="8962" max="8962" width="19.85546875" style="36" customWidth="1"/>
+    <col min="8963" max="8965" width="29.5703125" style="36" customWidth="1"/>
+    <col min="8966" max="8966" width="22.28515625" style="36" customWidth="1"/>
+    <col min="8967" max="8967" width="27.5703125" style="36" customWidth="1"/>
+    <col min="8968" max="8968" width="26.7109375" style="36" customWidth="1"/>
+    <col min="8969" max="8969" width="20.140625" style="36" customWidth="1"/>
+    <col min="8970" max="9217" width="8.7109375" style="36"/>
+    <col min="9218" max="9218" width="19.85546875" style="36" customWidth="1"/>
+    <col min="9219" max="9221" width="29.5703125" style="36" customWidth="1"/>
+    <col min="9222" max="9222" width="22.28515625" style="36" customWidth="1"/>
+    <col min="9223" max="9223" width="27.5703125" style="36" customWidth="1"/>
+    <col min="9224" max="9224" width="26.7109375" style="36" customWidth="1"/>
+    <col min="9225" max="9225" width="20.140625" style="36" customWidth="1"/>
+    <col min="9226" max="9473" width="8.7109375" style="36"/>
+    <col min="9474" max="9474" width="19.85546875" style="36" customWidth="1"/>
+    <col min="9475" max="9477" width="29.5703125" style="36" customWidth="1"/>
+    <col min="9478" max="9478" width="22.28515625" style="36" customWidth="1"/>
+    <col min="9479" max="9479" width="27.5703125" style="36" customWidth="1"/>
+    <col min="9480" max="9480" width="26.7109375" style="36" customWidth="1"/>
+    <col min="9481" max="9481" width="20.140625" style="36" customWidth="1"/>
+    <col min="9482" max="9729" width="8.7109375" style="36"/>
+    <col min="9730" max="9730" width="19.85546875" style="36" customWidth="1"/>
+    <col min="9731" max="9733" width="29.5703125" style="36" customWidth="1"/>
+    <col min="9734" max="9734" width="22.28515625" style="36" customWidth="1"/>
+    <col min="9735" max="9735" width="27.5703125" style="36" customWidth="1"/>
+    <col min="9736" max="9736" width="26.7109375" style="36" customWidth="1"/>
+    <col min="9737" max="9737" width="20.140625" style="36" customWidth="1"/>
+    <col min="9738" max="9985" width="8.7109375" style="36"/>
+    <col min="9986" max="9986" width="19.85546875" style="36" customWidth="1"/>
+    <col min="9987" max="9989" width="29.5703125" style="36" customWidth="1"/>
+    <col min="9990" max="9990" width="22.28515625" style="36" customWidth="1"/>
+    <col min="9991" max="9991" width="27.5703125" style="36" customWidth="1"/>
+    <col min="9992" max="9992" width="26.7109375" style="36" customWidth="1"/>
+    <col min="9993" max="9993" width="20.140625" style="36" customWidth="1"/>
+    <col min="9994" max="10241" width="8.7109375" style="36"/>
+    <col min="10242" max="10242" width="19.85546875" style="36" customWidth="1"/>
+    <col min="10243" max="10245" width="29.5703125" style="36" customWidth="1"/>
+    <col min="10246" max="10246" width="22.28515625" style="36" customWidth="1"/>
+    <col min="10247" max="10247" width="27.5703125" style="36" customWidth="1"/>
+    <col min="10248" max="10248" width="26.7109375" style="36" customWidth="1"/>
+    <col min="10249" max="10249" width="20.140625" style="36" customWidth="1"/>
+    <col min="10250" max="10497" width="8.7109375" style="36"/>
+    <col min="10498" max="10498" width="19.85546875" style="36" customWidth="1"/>
+    <col min="10499" max="10501" width="29.5703125" style="36" customWidth="1"/>
+    <col min="10502" max="10502" width="22.28515625" style="36" customWidth="1"/>
+    <col min="10503" max="10503" width="27.5703125" style="36" customWidth="1"/>
+    <col min="10504" max="10504" width="26.7109375" style="36" customWidth="1"/>
+    <col min="10505" max="10505" width="20.140625" style="36" customWidth="1"/>
+    <col min="10506" max="10753" width="8.7109375" style="36"/>
+    <col min="10754" max="10754" width="19.85546875" style="36" customWidth="1"/>
+    <col min="10755" max="10757" width="29.5703125" style="36" customWidth="1"/>
+    <col min="10758" max="10758" width="22.28515625" style="36" customWidth="1"/>
+    <col min="10759" max="10759" width="27.5703125" style="36" customWidth="1"/>
+    <col min="10760" max="10760" width="26.7109375" style="36" customWidth="1"/>
+    <col min="10761" max="10761" width="20.140625" style="36" customWidth="1"/>
+    <col min="10762" max="11009" width="8.7109375" style="36"/>
+    <col min="11010" max="11010" width="19.85546875" style="36" customWidth="1"/>
+    <col min="11011" max="11013" width="29.5703125" style="36" customWidth="1"/>
+    <col min="11014" max="11014" width="22.28515625" style="36" customWidth="1"/>
+    <col min="11015" max="11015" width="27.5703125" style="36" customWidth="1"/>
+    <col min="11016" max="11016" width="26.7109375" style="36" customWidth="1"/>
+    <col min="11017" max="11017" width="20.140625" style="36" customWidth="1"/>
+    <col min="11018" max="11265" width="8.7109375" style="36"/>
+    <col min="11266" max="11266" width="19.85546875" style="36" customWidth="1"/>
+    <col min="11267" max="11269" width="29.5703125" style="36" customWidth="1"/>
+    <col min="11270" max="11270" width="22.28515625" style="36" customWidth="1"/>
+    <col min="11271" max="11271" width="27.5703125" style="36" customWidth="1"/>
+    <col min="11272" max="11272" width="26.7109375" style="36" customWidth="1"/>
+    <col min="11273" max="11273" width="20.140625" style="36" customWidth="1"/>
+    <col min="11274" max="11521" width="8.7109375" style="36"/>
+    <col min="11522" max="11522" width="19.85546875" style="36" customWidth="1"/>
+    <col min="11523" max="11525" width="29.5703125" style="36" customWidth="1"/>
+    <col min="11526" max="11526" width="22.28515625" style="36" customWidth="1"/>
+    <col min="11527" max="11527" width="27.5703125" style="36" customWidth="1"/>
+    <col min="11528" max="11528" width="26.7109375" style="36" customWidth="1"/>
+    <col min="11529" max="11529" width="20.140625" style="36" customWidth="1"/>
+    <col min="11530" max="11777" width="8.7109375" style="36"/>
+    <col min="11778" max="11778" width="19.85546875" style="36" customWidth="1"/>
+    <col min="11779" max="11781" width="29.5703125" style="36" customWidth="1"/>
+    <col min="11782" max="11782" width="22.28515625" style="36" customWidth="1"/>
+    <col min="11783" max="11783" width="27.5703125" style="36" customWidth="1"/>
+    <col min="11784" max="11784" width="26.7109375" style="36" customWidth="1"/>
+    <col min="11785" max="11785" width="20.140625" style="36" customWidth="1"/>
+    <col min="11786" max="12033" width="8.7109375" style="36"/>
+    <col min="12034" max="12034" width="19.85546875" style="36" customWidth="1"/>
+    <col min="12035" max="12037" width="29.5703125" style="36" customWidth="1"/>
+    <col min="12038" max="12038" width="22.28515625" style="36" customWidth="1"/>
+    <col min="12039" max="12039" width="27.5703125" style="36" customWidth="1"/>
+    <col min="12040" max="12040" width="26.7109375" style="36" customWidth="1"/>
+    <col min="12041" max="12041" width="20.140625" style="36" customWidth="1"/>
+    <col min="12042" max="12289" width="8.7109375" style="36"/>
+    <col min="12290" max="12290" width="19.85546875" style="36" customWidth="1"/>
+    <col min="12291" max="12293" width="29.5703125" style="36" customWidth="1"/>
+    <col min="12294" max="12294" width="22.28515625" style="36" customWidth="1"/>
+    <col min="12295" max="12295" width="27.5703125" style="36" customWidth="1"/>
+    <col min="12296" max="12296" width="26.7109375" style="36" customWidth="1"/>
+    <col min="12297" max="12297" width="20.140625" style="36" customWidth="1"/>
+    <col min="12298" max="12545" width="8.7109375" style="36"/>
+    <col min="12546" max="12546" width="19.85546875" style="36" customWidth="1"/>
+    <col min="12547" max="12549" width="29.5703125" style="36" customWidth="1"/>
+    <col min="12550" max="12550" width="22.28515625" style="36" customWidth="1"/>
+    <col min="12551" max="12551" width="27.5703125" style="36" customWidth="1"/>
+    <col min="12552" max="12552" width="26.7109375" style="36" customWidth="1"/>
+    <col min="12553" max="12553" width="20.140625" style="36" customWidth="1"/>
+    <col min="12554" max="12801" width="8.7109375" style="36"/>
+    <col min="12802" max="12802" width="19.85546875" style="36" customWidth="1"/>
+    <col min="12803" max="12805" width="29.5703125" style="36" customWidth="1"/>
+    <col min="12806" max="12806" width="22.28515625" style="36" customWidth="1"/>
+    <col min="12807" max="12807" width="27.5703125" style="36" customWidth="1"/>
+    <col min="12808" max="12808" width="26.7109375" style="36" customWidth="1"/>
+    <col min="12809" max="12809" width="20.140625" style="36" customWidth="1"/>
+    <col min="12810" max="13057" width="8.7109375" style="36"/>
+    <col min="13058" max="13058" width="19.85546875" style="36" customWidth="1"/>
+    <col min="13059" max="13061" width="29.5703125" style="36" customWidth="1"/>
+    <col min="13062" max="13062" width="22.28515625" style="36" customWidth="1"/>
+    <col min="13063" max="13063" width="27.5703125" style="36" customWidth="1"/>
+    <col min="13064" max="13064" width="26.7109375" style="36" customWidth="1"/>
+    <col min="13065" max="13065" width="20.140625" style="36" customWidth="1"/>
+    <col min="13066" max="13313" width="8.7109375" style="36"/>
+    <col min="13314" max="13314" width="19.85546875" style="36" customWidth="1"/>
+    <col min="13315" max="13317" width="29.5703125" style="36" customWidth="1"/>
+    <col min="13318" max="13318" width="22.28515625" style="36" customWidth="1"/>
+    <col min="13319" max="13319" width="27.5703125" style="36" customWidth="1"/>
+    <col min="13320" max="13320" width="26.7109375" style="36" customWidth="1"/>
+    <col min="13321" max="13321" width="20.140625" style="36" customWidth="1"/>
+    <col min="13322" max="13569" width="8.7109375" style="36"/>
+    <col min="13570" max="13570" width="19.85546875" style="36" customWidth="1"/>
+    <col min="13571" max="13573" width="29.5703125" style="36" customWidth="1"/>
+    <col min="13574" max="13574" width="22.28515625" style="36" customWidth="1"/>
+    <col min="13575" max="13575" width="27.5703125" style="36" customWidth="1"/>
+    <col min="13576" max="13576" width="26.7109375" style="36" customWidth="1"/>
+    <col min="13577" max="13577" width="20.140625" style="36" customWidth="1"/>
+    <col min="13578" max="13825" width="8.7109375" style="36"/>
+    <col min="13826" max="13826" width="19.85546875" style="36" customWidth="1"/>
+    <col min="13827" max="13829" width="29.5703125" style="36" customWidth="1"/>
+    <col min="13830" max="13830" width="22.28515625" style="36" customWidth="1"/>
+    <col min="13831" max="13831" width="27.5703125" style="36" customWidth="1"/>
+    <col min="13832" max="13832" width="26.7109375" style="36" customWidth="1"/>
+    <col min="13833" max="13833" width="20.140625" style="36" customWidth="1"/>
+    <col min="13834" max="14081" width="8.7109375" style="36"/>
+    <col min="14082" max="14082" width="19.85546875" style="36" customWidth="1"/>
+    <col min="14083" max="14085" width="29.5703125" style="36" customWidth="1"/>
+    <col min="14086" max="14086" width="22.28515625" style="36" customWidth="1"/>
+    <col min="14087" max="14087" width="27.5703125" style="36" customWidth="1"/>
+    <col min="14088" max="14088" width="26.7109375" style="36" customWidth="1"/>
+    <col min="14089" max="14089" width="20.140625" style="36" customWidth="1"/>
+    <col min="14090" max="14337" width="8.7109375" style="36"/>
+    <col min="14338" max="14338" width="19.85546875" style="36" customWidth="1"/>
+    <col min="14339" max="14341" width="29.5703125" style="36" customWidth="1"/>
+    <col min="14342" max="14342" width="22.28515625" style="36" customWidth="1"/>
+    <col min="14343" max="14343" width="27.5703125" style="36" customWidth="1"/>
+    <col min="14344" max="14344" width="26.7109375" style="36" customWidth="1"/>
+    <col min="14345" max="14345" width="20.140625" style="36" customWidth="1"/>
+    <col min="14346" max="14593" width="8.7109375" style="36"/>
+    <col min="14594" max="14594" width="19.85546875" style="36" customWidth="1"/>
+    <col min="14595" max="14597" width="29.5703125" style="36" customWidth="1"/>
+    <col min="14598" max="14598" width="22.28515625" style="36" customWidth="1"/>
+    <col min="14599" max="14599" width="27.5703125" style="36" customWidth="1"/>
+    <col min="14600" max="14600" width="26.7109375" style="36" customWidth="1"/>
+    <col min="14601" max="14601" width="20.140625" style="36" customWidth="1"/>
+    <col min="14602" max="14849" width="8.7109375" style="36"/>
+    <col min="14850" max="14850" width="19.85546875" style="36" customWidth="1"/>
+    <col min="14851" max="14853" width="29.5703125" style="36" customWidth="1"/>
+    <col min="14854" max="14854" width="22.28515625" style="36" customWidth="1"/>
+    <col min="14855" max="14855" width="27.5703125" style="36" customWidth="1"/>
+    <col min="14856" max="14856" width="26.7109375" style="36" customWidth="1"/>
+    <col min="14857" max="14857" width="20.140625" style="36" customWidth="1"/>
+    <col min="14858" max="15105" width="8.7109375" style="36"/>
+    <col min="15106" max="15106" width="19.85546875" style="36" customWidth="1"/>
+    <col min="15107" max="15109" width="29.5703125" style="36" customWidth="1"/>
+    <col min="15110" max="15110" width="22.28515625" style="36" customWidth="1"/>
+    <col min="15111" max="15111" width="27.5703125" style="36" customWidth="1"/>
+    <col min="15112" max="15112" width="26.7109375" style="36" customWidth="1"/>
+    <col min="15113" max="15113" width="20.140625" style="36" customWidth="1"/>
+    <col min="15114" max="15361" width="8.7109375" style="36"/>
+    <col min="15362" max="15362" width="19.85546875" style="36" customWidth="1"/>
+    <col min="15363" max="15365" width="29.5703125" style="36" customWidth="1"/>
+    <col min="15366" max="15366" width="22.28515625" style="36" customWidth="1"/>
+    <col min="15367" max="15367" width="27.5703125" style="36" customWidth="1"/>
+    <col min="15368" max="15368" width="26.7109375" style="36" customWidth="1"/>
+    <col min="15369" max="15369" width="20.140625" style="36" customWidth="1"/>
+    <col min="15370" max="15617" width="8.7109375" style="36"/>
+    <col min="15618" max="15618" width="19.85546875" style="36" customWidth="1"/>
+    <col min="15619" max="15621" width="29.5703125" style="36" customWidth="1"/>
+    <col min="15622" max="15622" width="22.28515625" style="36" customWidth="1"/>
+    <col min="15623" max="15623" width="27.5703125" style="36" customWidth="1"/>
+    <col min="15624" max="15624" width="26.7109375" style="36" customWidth="1"/>
+    <col min="15625" max="15625" width="20.140625" style="36" customWidth="1"/>
+    <col min="15626" max="15873" width="8.7109375" style="36"/>
+    <col min="15874" max="15874" width="19.85546875" style="36" customWidth="1"/>
+    <col min="15875" max="15877" width="29.5703125" style="36" customWidth="1"/>
+    <col min="15878" max="15878" width="22.28515625" style="36" customWidth="1"/>
+    <col min="15879" max="15879" width="27.5703125" style="36" customWidth="1"/>
+    <col min="15880" max="15880" width="26.7109375" style="36" customWidth="1"/>
+    <col min="15881" max="15881" width="20.140625" style="36" customWidth="1"/>
+    <col min="15882" max="16129" width="8.7109375" style="36"/>
+    <col min="16130" max="16130" width="19.85546875" style="36" customWidth="1"/>
+    <col min="16131" max="16133" width="29.5703125" style="36" customWidth="1"/>
+    <col min="16134" max="16134" width="22.28515625" style="36" customWidth="1"/>
+    <col min="16135" max="16135" width="27.5703125" style="36" customWidth="1"/>
+    <col min="16136" max="16136" width="26.7109375" style="36" customWidth="1"/>
+    <col min="16137" max="16137" width="20.140625" style="36" customWidth="1"/>
+    <col min="16138" max="16384" width="8.7109375" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="36" t="s">
         <v>410</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="36" t="s">
         <v>411</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="36" t="s">
         <v>412</v>
       </c>
-      <c r="F3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
+      <c r="F3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="46">
-        <v>0</v>
-      </c>
-      <c r="B4" s="46" t="s">
+      <c r="A4" s="36">
+        <v>0</v>
+      </c>
+      <c r="B4" s="36" t="s">
         <v>413</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="F4" s="49"/>
+      <c r="F4" s="38"/>
       <c r="G4"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="46">
-        <v>1</v>
-      </c>
-      <c r="B5" s="46" t="s">
+      <c r="A5" s="36">
+        <v>1</v>
+      </c>
+      <c r="B5" s="36" t="s">
         <v>414</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="46" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="F5" s="49"/>
+      <c r="F5" s="38"/>
       <c r="G5"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="46">
-        <v>2</v>
-      </c>
-      <c r="B6" s="46" t="s">
+      <c r="A6" s="36">
+        <v>2</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>415</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="46" t="s">
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="F6" s="49"/>
+      <c r="F6" s="38"/>
       <c r="G6"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="46">
-        <v>3</v>
-      </c>
-      <c r="B7" s="46" t="s">
+      <c r="A7" s="36">
+        <v>3</v>
+      </c>
+      <c r="B7" s="36" t="s">
         <v>416</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="36" t="s">
         <v>417</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="36" t="s">
         <v>418</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="36" t="s">
         <v>177</v>
       </c>
       <c r="G7"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="46">
+      <c r="A8" s="36">
         <v>4</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="36" t="s">
         <v>419</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="36" t="s">
         <v>420</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="36" t="s">
         <v>418</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="36" t="s">
         <v>179</v>
       </c>
       <c r="G8"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="46">
+      <c r="A9" s="36">
         <v>5</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="36" t="s">
         <v>421</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="36" t="s">
         <v>422</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="36" t="s">
         <v>423</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="36" t="s">
         <v>180</v>
       </c>
       <c r="G9"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="46">
+      <c r="A10" s="36">
         <v>6</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="36" t="s">
         <v>424</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="36" t="s">
         <v>425</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="36" t="s">
         <v>426</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="36" t="s">
         <v>182</v>
       </c>
       <c r="G10"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="46">
+      <c r="A11" s="36">
         <v>7</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="36" t="s">
         <v>427</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="36" t="s">
         <v>428</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E11" s="36" t="s">
         <v>184</v>
       </c>
       <c r="G11"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="36" t="s">
         <v>415</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="36" t="s">
         <v>414</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="36" t="s">
         <v>430</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="41" t="s">
         <v>431</v>
       </c>
-      <c r="F16" s="53"/>
-      <c r="G16" s="47"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="50">
-        <v>0</v>
-      </c>
-      <c r="C17" s="50">
-        <v>0</v>
-      </c>
-      <c r="D17" s="50">
-        <v>0</v>
-      </c>
-      <c r="E17" s="50" t="s">
+      <c r="B17" s="39">
+        <v>0</v>
+      </c>
+      <c r="C17" s="39">
+        <v>0</v>
+      </c>
+      <c r="D17" s="39">
+        <v>0</v>
+      </c>
+      <c r="E17" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="50">
-        <v>0</v>
-      </c>
-      <c r="C18" s="50">
-        <v>0</v>
-      </c>
-      <c r="D18" s="50">
-        <v>1</v>
-      </c>
-      <c r="E18" s="50" t="s">
+      <c r="B18" s="39">
+        <v>0</v>
+      </c>
+      <c r="C18" s="39">
+        <v>0</v>
+      </c>
+      <c r="D18" s="39">
+        <v>1</v>
+      </c>
+      <c r="E18" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="50">
-        <v>0</v>
-      </c>
-      <c r="C19" s="50">
-        <v>1</v>
-      </c>
-      <c r="D19" s="50">
-        <v>0</v>
-      </c>
-      <c r="E19" s="50" t="s">
+      <c r="B19" s="39">
+        <v>0</v>
+      </c>
+      <c r="C19" s="39">
+        <v>1</v>
+      </c>
+      <c r="D19" s="39">
+        <v>0</v>
+      </c>
+      <c r="E19" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="50">
-        <v>0</v>
-      </c>
-      <c r="C20" s="50">
-        <v>1</v>
-      </c>
-      <c r="D20" s="50">
-        <v>1</v>
-      </c>
-      <c r="E20" s="50" t="s">
+      <c r="B20" s="39">
+        <v>0</v>
+      </c>
+      <c r="C20" s="39">
+        <v>1</v>
+      </c>
+      <c r="D20" s="39">
+        <v>1</v>
+      </c>
+      <c r="E20" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="50">
-        <v>1</v>
-      </c>
-      <c r="C21" s="50">
-        <v>0</v>
-      </c>
-      <c r="D21" s="50">
-        <v>0</v>
-      </c>
-      <c r="E21" s="50" t="s">
+      <c r="B21" s="39">
+        <v>1</v>
+      </c>
+      <c r="C21" s="39">
+        <v>0</v>
+      </c>
+      <c r="D21" s="39">
+        <v>0</v>
+      </c>
+      <c r="E21" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="50">
-        <v>1</v>
-      </c>
-      <c r="C22" s="50">
-        <v>0</v>
-      </c>
-      <c r="D22" s="50">
-        <v>1</v>
-      </c>
-      <c r="E22" s="50" t="s">
+      <c r="B22" s="39">
+        <v>1</v>
+      </c>
+      <c r="C22" s="39">
+        <v>0</v>
+      </c>
+      <c r="D22" s="39">
+        <v>1</v>
+      </c>
+      <c r="E22" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="50">
-        <v>1</v>
-      </c>
-      <c r="C23" s="50">
-        <v>1</v>
-      </c>
-      <c r="D23" s="50">
-        <v>0</v>
-      </c>
-      <c r="E23" s="50" t="s">
+      <c r="B23" s="39">
+        <v>1</v>
+      </c>
+      <c r="C23" s="39">
+        <v>1</v>
+      </c>
+      <c r="D23" s="39">
+        <v>0</v>
+      </c>
+      <c r="E23" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="50">
-        <v>1</v>
-      </c>
-      <c r="C24" s="50">
-        <v>1</v>
-      </c>
-      <c r="D24" s="50">
-        <v>1</v>
-      </c>
-      <c r="E24" s="50" t="s">
+      <c r="B24" s="39">
+        <v>1</v>
+      </c>
+      <c r="C24" s="39">
+        <v>1</v>
+      </c>
+      <c r="D24" s="39">
+        <v>1</v>
+      </c>
+      <c r="E24" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -37233,15 +37263,15 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="49" t="s">
         <v>394</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>393</v>
       </c>
-      <c r="G2" s="45"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="35" t="s">
         <v>392</v>
       </c>
@@ -37259,19 +37289,19 @@
       <c r="C3" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="49" t="s">
         <v>385</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="49" t="s">
         <v>384</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="50" t="s">
         <v>383</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="50" t="s">
         <v>382</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="51" t="s">
         <v>381</v>
       </c>
     </row>
@@ -37285,11 +37315,11 @@
       <c r="C4" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="43"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="51"/>
       <c r="K4" s="30"/>
       <c r="L4" s="30"/>
       <c r="M4" s="30"/>
@@ -37305,11 +37335,11 @@
       <c r="C5" s="34" t="s">
         <v>375</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="43"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="51"/>
       <c r="J5" s="28" t="s">
         <v>391</v>
       </c>
@@ -37328,11 +37358,11 @@
       <c r="C6" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="43"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="51"/>
       <c r="K6" s="30"/>
       <c r="L6" s="30"/>
       <c r="M6" s="30"/>
@@ -37348,19 +37378,19 @@
       <c r="C7" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="49" t="s">
         <v>377</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="52" t="s">
         <v>370</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="50" t="s">
         <v>376</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="50" t="s">
         <v>375</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="51" t="s">
         <v>374</v>
       </c>
       <c r="K7" s="30"/>
@@ -37378,11 +37408,11 @@
       <c r="C8" s="34" t="s">
         <v>372</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="43"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="51"/>
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -37399,11 +37429,11 @@
       <c r="C9" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="43"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="51"/>
       <c r="J9" s="30"/>
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
@@ -37420,11 +37450,11 @@
       <c r="C10" s="34" t="s">
         <v>368</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="43"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="51"/>
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
@@ -37432,15 +37462,15 @@
       <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="53" t="s">
         <v>390</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="42" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54" t="s">
         <v>389</v>
       </c>
-      <c r="G11" s="42"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="33" t="s">
         <v>388</v>
       </c>
@@ -37462,19 +37492,19 @@
       <c r="C12" s="32" t="s">
         <v>386</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="53" t="s">
         <v>385</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="53" t="s">
         <v>384</v>
       </c>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="54" t="s">
         <v>383</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="54" t="s">
         <v>382</v>
       </c>
-      <c r="H12" s="39" t="s">
+      <c r="H12" s="55" t="s">
         <v>381</v>
       </c>
       <c r="K12" s="30"/>
@@ -37492,11 +37522,11 @@
       <c r="C13" s="32" t="s">
         <v>380</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="39"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="55"/>
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
       <c r="M13" s="30"/>
@@ -37512,11 +37542,11 @@
       <c r="C14" s="32" t="s">
         <v>375</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="39"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="55"/>
       <c r="K14" s="30"/>
       <c r="L14" s="30"/>
       <c r="M14" s="30"/>
@@ -37532,11 +37562,11 @@
       <c r="C15" s="32" t="s">
         <v>376</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="39"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="55"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
@@ -37552,19 +37582,19 @@
       <c r="C16" s="32" t="s">
         <v>378</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="53" t="s">
         <v>377</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="52" t="s">
         <v>370</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="54" t="s">
         <v>376</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="54" t="s">
         <v>375</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="55" t="s">
         <v>374</v>
       </c>
       <c r="K16" s="30"/>
@@ -37582,11 +37612,11 @@
       <c r="C17" s="32" t="s">
         <v>372</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="39"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="55"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
       <c r="M17" s="30"/>
@@ -37602,11 +37632,11 @@
       <c r="C18" s="32" t="s">
         <v>370</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="39"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="55"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
       <c r="M18" s="30"/>
@@ -37622,11 +37652,11 @@
       <c r="C19" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="39"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="55"/>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
@@ -37685,30 +37715,30 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="24">
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="G3:G6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>